<commit_message>
updates to benchmark results
</commit_message>
<xml_diff>
--- a/verilog/hardware/processor/source/instruction_counts.xlsx
+++ b/verilog/hardware/processor/source/instruction_counts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\f-of-e-tools\verilog\hardware\processor\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC6FDCC-699A-45F9-81B7-745D726B8882}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4443D8C0-0CC2-4C52-ADD1-F9F187773130}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instruction_counts" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="140">
   <si>
     <t>LUI</t>
   </si>
@@ -470,6 +470,9 @@
   </si>
   <si>
     <t>execution frequency on hardware at 12MHz</t>
+  </si>
+  <si>
+    <t>average CPI on hardware at 12MHz</t>
   </si>
 </sst>
 </file>
@@ -1323,13 +1326,13 @@
   <dimension ref="A1:AB80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="42.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" hidden="1" customWidth="1"/>
     <col min="3" max="10" width="20.28515625" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1583,10 +1586,6 @@
       <c r="A9" t="s">
         <v>114</v>
       </c>
-      <c r="C9" t="e">
-        <f>C3/(C8*6000000)</f>
-        <v>#DIV/0!</v>
-      </c>
       <c r="D9">
         <f>6000000/(D8*D3)</f>
         <v>4.6583380034465796</v>
@@ -1625,12 +1624,15 @@
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>139</v>
+      </c>
       <c r="D11">
         <f>12000000/(D10*D3)</f>
         <v>4.6581153401894007</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>137</v>
       </c>
@@ -1667,7 +1669,8 @@
         <v>2.3471637738776292</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>109</v>
       </c>
@@ -1675,7 +1678,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
Added dynamic power measurements
</commit_message>
<xml_diff>
--- a/verilog/hardware/processor/source/instruction_counts.xlsx
+++ b/verilog/hardware/processor/source/instruction_counts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\f-of-e-tools\verilog\hardware\processor\source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcos/GB3/f-of-e-tools/verilog/hardware/processor/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4443D8C0-0CC2-4C52-ADD1-F9F187773130}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B599D4B-8EA3-384B-B85D-527A250A04B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instruction_counts" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="141">
   <si>
     <t>LUI</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t>average CPI on hardware at 12MHz</t>
+  </si>
+  <si>
+    <t>Average Dynamic Power</t>
   </si>
 </sst>
 </file>
@@ -1323,21 +1326,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB80"/>
+  <dimension ref="A1:AB81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" hidden="1" customWidth="1"/>
-    <col min="3" max="10" width="20.28515625" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.5" hidden="1" customWidth="1"/>
+    <col min="3" max="10" width="20.33203125" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>98</v>
       </c>
@@ -1366,7 +1369,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -1395,7 +1398,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -1424,7 +1427,7 @@
         <v>148383</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -1453,7 +1456,7 @@
         <v>210219</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>111</v>
       </c>
@@ -1482,7 +1485,7 @@
         <v>159639</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>133</v>
       </c>
@@ -1519,7 +1522,7 @@
         <v>61836</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -1556,7 +1559,7 @@
         <v>1.4167323750025271</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -1582,7 +1585,7 @@
         <v>18.149000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -1615,7 +1618,7 @@
         <v>2.2279959772507749</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>138</v>
       </c>
@@ -1623,7 +1626,7 @@
         <v>20.920999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>139</v>
       </c>
@@ -1632,1832 +1635,1829 @@
         <v>4.6581153401894007</v>
       </c>
     </row>
-    <row r="13" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12">
+        <v>2.8623899999999998E-3</v>
+      </c>
+      <c r="D12">
+        <v>3.8369400000000001E-3</v>
+      </c>
+      <c r="E12">
+        <v>3.9933499999999997E-3</v>
+      </c>
+      <c r="F12">
+        <v>4.0100099999999996E-3</v>
+      </c>
+      <c r="G12">
+        <v>4.0216200000000001E-3</v>
+      </c>
+      <c r="H12">
+        <v>4.1289200000000003E-3</v>
+      </c>
+      <c r="I12">
+        <v>4.0061000000000003E-3</v>
+      </c>
+      <c r="J12">
+        <v>4.0835200000000002E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>137</v>
       </c>
-      <c r="C13">
-        <f>(C4-C18*$B18-C19*$B19-C20*$B20-C21*$B21-C22*$B22-C23*$B23)/C17</f>
+      <c r="C14">
+        <f>(C4-C19*$B19-C20*$B20-C21*$B21-C22*$B22-C23*$B23-C24*$B24)/C18</f>
         <v>2.7175042348955398</v>
       </c>
-      <c r="D13">
-        <f t="shared" ref="D13:J13" si="3">(D4-D18*$B18-D19*$B19-D20*$B20-D21*$B21-D22*$B22-D23*$B23)/D17</f>
+      <c r="D14">
+        <f t="shared" ref="D14:J14" si="3">(D4-D19*$B19-D20*$B20-D21*$B21-D22*$B22-D23*$B23-D24*$B24)/D18</f>
         <v>2.8716495570243268</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <f t="shared" si="3"/>
         <v>2.8593758707160766</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <f t="shared" si="3"/>
         <v>2.8720933502038517</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <f t="shared" si="3"/>
         <v>2.9329911404865703</v>
       </c>
-      <c r="H13">
+      <c r="H14">
         <f t="shared" si="3"/>
         <v>4.0255012260204817</v>
       </c>
-      <c r="I13">
+      <c r="I14">
         <f t="shared" si="3"/>
         <v>3.4167411894802631</v>
       </c>
-      <c r="J13">
+      <c r="J14">
         <f t="shared" si="3"/>
         <v>2.3471637738776292</v>
       </c>
     </row>
-    <row r="14" spans="1:28" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>109</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>104</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>136</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L17" t="s">
         <v>120</v>
       </c>
-      <c r="S16" t="s">
+      <c r="S17" t="s">
         <v>121</v>
       </c>
-      <c r="U16" t="s">
+      <c r="U17" t="s">
         <v>122</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AB17" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>116</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>135</v>
       </c>
-      <c r="C17">
-        <f>SUM(C30:C35)</f>
+      <c r="C18">
+        <f>SUM(C31:C36)</f>
         <v>3542</v>
       </c>
-      <c r="D17">
-        <f t="shared" ref="D17:J17" si="4">SUM(D30:D35)</f>
+      <c r="D18">
+        <f t="shared" ref="D18:J18" si="4">SUM(D31:D36)</f>
         <v>7111</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <f t="shared" si="4"/>
         <v>10767</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <f t="shared" si="4"/>
         <v>7113</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <f t="shared" si="4"/>
         <v>7111</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <f t="shared" si="4"/>
         <v>20799</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <f t="shared" si="4"/>
         <v>20799</v>
       </c>
-      <c r="J17">
+      <c r="J18">
         <f t="shared" si="4"/>
         <v>10313</v>
       </c>
-      <c r="L17" cm="1">
-        <f t="array" ref="L17:R23">TRANSPOSE(D17:J23)</f>
+      <c r="L18" cm="1">
+        <f t="array" ref="L18:R24">TRANSPOSE(D18:J24)</f>
         <v>7111</v>
       </c>
-      <c r="M17">
+      <c r="M18">
         <v>32838</v>
       </c>
-      <c r="N17">
+      <c r="N18">
         <v>66218</v>
       </c>
-      <c r="O17">
+      <c r="O18">
         <v>8076</v>
       </c>
-      <c r="P17">
+      <c r="P18">
         <v>8754</v>
       </c>
-      <c r="Q17">
+      <c r="Q18">
         <v>136</v>
       </c>
-      <c r="R17">
-        <v>1</v>
-      </c>
-      <c r="S17" cm="1">
-        <f t="array" ref="S17:S23">TRANSPOSE(D4:J4)</f>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18" cm="1">
+        <f t="array" ref="S18:S24">TRANSPOSE(D4:J4)</f>
         <v>180167</v>
       </c>
-      <c r="U17" cm="1">
-        <f t="array" ref="U17:AA23">MINVERSE(_xlfn.ANCHORARRAY(L17))</f>
+      <c r="U18" cm="1">
+        <f t="array" ref="U18:AA24">MINVERSE(_xlfn.ANCHORARRAY(L18))</f>
         <v>-3.635087081951479E-2</v>
       </c>
-      <c r="V17">
+      <c r="V18">
         <v>3.3922861115084674E-4</v>
       </c>
-      <c r="W17">
+      <c r="W18">
         <v>3.6263097317328408E-2</v>
       </c>
-      <c r="X17">
+      <c r="X18">
         <v>-8.537532976016373E-5</v>
       </c>
-      <c r="Y17">
+      <c r="Y18">
         <v>7.4902649042440746E-5</v>
       </c>
-      <c r="Z17">
+      <c r="Z18">
         <v>-5.4013706069903682E-5</v>
       </c>
-      <c r="AA17">
+      <c r="AA18">
         <v>-1.8696872217683933E-4</v>
       </c>
-      <c r="AB17" cm="1">
-        <f t="array" ref="AB17:AB23">MMULT(_xlfn.ANCHORARRAY(U17),_xlfn.ANCHORARRAY(S17))</f>
+      <c r="AB18" cm="1">
+        <f t="array" ref="AB18:AB24">MMULT(_xlfn.ANCHORARRAY(U18),_xlfn.ANCHORARRAY(S18))</f>
         <v>5.1005820389660883</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>56</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <f>SUM(C53,C44,C54)</f>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <f>SUM(C54,C45,C55)</f>
         <v>26340</v>
       </c>
-      <c r="D18">
-        <f t="shared" ref="D18:J18" si="5">SUM(D53,D44,D54)</f>
+      <c r="D19">
+        <f t="shared" ref="D19:J19" si="5">SUM(D54,D45,D55)</f>
         <v>32838</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <f t="shared" si="5"/>
         <v>36380</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <f t="shared" si="5"/>
         <v>32838</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <f t="shared" si="5"/>
         <v>70642</v>
       </c>
-      <c r="H18">
+      <c r="H19">
         <f t="shared" si="5"/>
         <v>114964</v>
       </c>
-      <c r="I18">
+      <c r="I19">
         <f t="shared" si="5"/>
         <v>73902</v>
       </c>
-      <c r="J18">
+      <c r="J19">
         <f t="shared" si="5"/>
         <v>43040</v>
       </c>
-      <c r="L18">
+      <c r="L19">
         <v>10767</v>
       </c>
-      <c r="M18">
+      <c r="M19">
         <v>36380</v>
       </c>
-      <c r="N18">
+      <c r="N19">
         <v>76950</v>
       </c>
-      <c r="O18">
+      <c r="O19">
         <v>11732</v>
       </c>
-      <c r="P18">
+      <c r="P19">
         <v>8754</v>
       </c>
-      <c r="Q18">
+      <c r="Q19">
         <v>254</v>
       </c>
-      <c r="R18">
-        <v>1</v>
-      </c>
-      <c r="S18">
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
         <v>216495</v>
       </c>
-      <c r="U18">
+      <c r="U19">
         <v>3.9324532784843887E-2</v>
       </c>
-      <c r="V18">
+      <c r="V19">
         <v>-1.7838593987774123E-4</v>
       </c>
-      <c r="W18">
+      <c r="W19">
         <v>-3.933382198221004E-2</v>
       </c>
-      <c r="X18">
+      <c r="X19">
         <v>7.3872310242267076E-6</v>
       </c>
-      <c r="Y18">
+      <c r="Y19">
         <v>-2.2860238881440793E-5</v>
       </c>
-      <c r="Z18">
+      <c r="Z19">
         <v>3.750498086523561E-5</v>
       </c>
-      <c r="AA18">
+      <c r="AA19">
         <v>1.6564316423587071E-4</v>
       </c>
-      <c r="AB18">
+      <c r="AB19">
         <v>-0.11675093523181346</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>117</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>1.55</v>
       </c>
-      <c r="C19">
-        <f>SUM(C36:C40)</f>
+      <c r="C20">
+        <f>SUM(C37:C41)</f>
         <v>23130</v>
       </c>
-      <c r="D19">
-        <f t="shared" ref="D19:J19" si="6">SUM(D36:D40)</f>
+      <c r="D20">
+        <f t="shared" ref="D20:J20" si="6">SUM(D37:D41)</f>
         <v>66218</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <f t="shared" si="6"/>
         <v>76950</v>
       </c>
-      <c r="F19">
+      <c r="F20">
         <f t="shared" si="6"/>
         <v>66220</v>
       </c>
-      <c r="G19">
+      <c r="G20">
         <f t="shared" si="6"/>
         <v>136010</v>
       </c>
-      <c r="H19">
+      <c r="H20">
         <f t="shared" si="6"/>
         <v>165454</v>
       </c>
-      <c r="I19">
+      <c r="I20">
         <f t="shared" si="6"/>
         <v>148346</v>
       </c>
-      <c r="J19">
+      <c r="J20">
         <f t="shared" si="6"/>
         <v>70238</v>
       </c>
-      <c r="L19">
+      <c r="L20">
         <v>7113</v>
       </c>
-      <c r="M19">
+      <c r="M20">
         <v>32838</v>
       </c>
-      <c r="N19">
+      <c r="N20">
         <v>66220</v>
       </c>
-      <c r="O19">
+      <c r="O20">
         <v>8076</v>
       </c>
-      <c r="P19">
+      <c r="P20">
         <v>8754</v>
       </c>
-      <c r="Q19">
+      <c r="Q20">
         <v>138</v>
       </c>
-      <c r="R19">
-        <v>1</v>
-      </c>
-      <c r="S19">
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
         <v>180181</v>
       </c>
-      <c r="U19">
+      <c r="U20">
         <v>-1.361724196571419E-2</v>
       </c>
-      <c r="V19">
+      <c r="V20">
         <v>3.26543015085874E-5</v>
       </c>
-      <c r="W19">
+      <c r="W20">
         <v>1.3624344241461816E-2</v>
       </c>
-      <c r="X19">
+      <c r="X20">
         <v>1.0534513201513464E-5</v>
       </c>
-      <c r="Y19">
+      <c r="Y20">
         <v>-1.0525039752714027E-6</v>
       </c>
-      <c r="Z19">
+      <c r="Z20">
         <v>2.4256926885382997E-6</v>
       </c>
-      <c r="AA19">
+      <c r="AA20">
         <v>-5.1664279170991959E-5</v>
       </c>
-      <c r="AB19">
+      <c r="AB20">
         <v>1.8749830109410635</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>118</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>1.55</v>
       </c>
-      <c r="C20">
-        <f>SUM(C41:C43)</f>
+      <c r="C21">
+        <f>SUM(C42:C44)</f>
         <v>4022</v>
       </c>
-      <c r="D20">
-        <f t="shared" ref="D20:J20" si="7">SUM(D41:D43)</f>
+      <c r="D21">
+        <f t="shared" ref="D21:J21" si="7">SUM(D42:D44)</f>
         <v>8076</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <f t="shared" si="7"/>
         <v>11732</v>
       </c>
-      <c r="F20">
+      <c r="F21">
         <f t="shared" si="7"/>
         <v>8076</v>
       </c>
-      <c r="G20">
+      <c r="G21">
         <f t="shared" si="7"/>
         <v>16800</v>
       </c>
-      <c r="H20">
+      <c r="H21">
         <f t="shared" si="7"/>
         <v>11498</v>
       </c>
-      <c r="I20">
+      <c r="I21">
         <f t="shared" si="7"/>
         <v>8078</v>
       </c>
-      <c r="J20">
+      <c r="J21">
         <f t="shared" si="7"/>
         <v>12096</v>
       </c>
-      <c r="L20">
+      <c r="L21">
         <v>7111</v>
       </c>
-      <c r="M20">
+      <c r="M21">
         <v>70642</v>
       </c>
-      <c r="N20">
+      <c r="N21">
         <v>136010</v>
       </c>
-      <c r="O20">
+      <c r="O21">
         <v>16800</v>
       </c>
-      <c r="P20">
+      <c r="P21">
         <v>26202</v>
       </c>
-      <c r="Q20">
+      <c r="Q21">
         <v>136</v>
       </c>
-      <c r="R20">
-        <v>1</v>
-      </c>
-      <c r="S20">
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21">
         <v>357555</v>
       </c>
-      <c r="U20">
+      <c r="U21">
         <v>5.2476830432061736E-2</v>
       </c>
-      <c r="V20">
+      <c r="V21">
         <v>2.3265704754675745E-5</v>
       </c>
-      <c r="W20">
+      <c r="W21">
         <v>-5.2677032447099745E-2</v>
       </c>
-      <c r="X20">
+      <c r="X21">
         <v>4.4879382188945695E-5</v>
       </c>
-      <c r="Y20">
+      <c r="Y21">
         <v>-4.7282092177396974E-5</v>
       </c>
-      <c r="Z20">
+      <c r="Z21">
         <v>8.8926552665522262E-6</v>
       </c>
-      <c r="AA20">
+      <c r="AA21">
         <v>1.7044636500523016E-4</v>
       </c>
-      <c r="AB20">
+      <c r="AB21">
         <v>-0.55563378539225283</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>126</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <f>SUM(C49,C58,C59:C62,C50:C52,C55,C26)</f>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <f>SUM(C50,C59,C60:C63,C51:C53,C56,C27)</f>
         <v>14329</v>
       </c>
-      <c r="D21">
-        <f t="shared" ref="D21:J21" si="8">SUM(D49,D58,D59:D62,D50:D52,D55)</f>
+      <c r="D22">
+        <f t="shared" ref="D22:J22" si="8">SUM(D50,D59,D60:D63,D51:D53,D56)</f>
         <v>8754</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <f t="shared" si="8"/>
         <v>8754</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <f t="shared" si="8"/>
         <v>8754</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <f t="shared" si="8"/>
         <v>26202</v>
       </c>
-      <c r="H21">
+      <c r="H22">
         <f t="shared" si="8"/>
         <v>36130</v>
       </c>
-      <c r="I21">
+      <c r="I22">
         <f t="shared" si="8"/>
         <v>8754</v>
       </c>
-      <c r="J21">
+      <c r="J22">
         <f t="shared" si="8"/>
         <v>11754</v>
       </c>
-      <c r="L21">
+      <c r="L22">
         <v>20799</v>
       </c>
-      <c r="M21">
+      <c r="M22">
         <v>114964</v>
       </c>
-      <c r="N21">
+      <c r="N22">
         <v>165454</v>
       </c>
-      <c r="O21">
+      <c r="O22">
         <v>11498</v>
       </c>
-      <c r="P21">
+      <c r="P22">
         <v>36130</v>
       </c>
-      <c r="Q21">
+      <c r="Q22">
         <v>136</v>
       </c>
-      <c r="R21">
-        <v>1</v>
-      </c>
-      <c r="S21">
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22">
         <v>512095</v>
       </c>
-      <c r="U21">
+      <c r="U22">
         <v>-5.7029914879437184E-2</v>
       </c>
-      <c r="V21">
+      <c r="V22">
         <v>2.4425281132341858E-4</v>
       </c>
-      <c r="W21">
+      <c r="W22">
         <v>5.7064420219157697E-2</v>
       </c>
-      <c r="X21">
+      <c r="X22">
         <v>-2.3270252018354897E-5</v>
       </c>
-      <c r="Y21">
+      <c r="Y22">
         <v>7.738157956623914E-5</v>
       </c>
-      <c r="Z21">
+      <c r="Z22">
         <v>-9.5409890262106474E-5</v>
       </c>
-      <c r="AA21">
+      <c r="AA22">
         <v>-2.3745958832970047E-4</v>
       </c>
-      <c r="AB21">
+      <c r="AB22">
         <v>3.197511875270358</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>124</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <f>SUM(C28:C29, C27,C63:C66,C56:C57)</f>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <f>SUM(C29:C30, C28,C64:C67,C57:C58)</f>
         <v>67</v>
       </c>
-      <c r="D22">
-        <f t="shared" ref="D22:J22" si="9">SUM(D28:D29, D27,D63:D66,D56:D57)</f>
+      <c r="D23">
+        <f t="shared" ref="D23:J23" si="9">SUM(D29:D30, D28,D64:D67,D57:D58)</f>
         <v>136</v>
       </c>
-      <c r="E22">
+      <c r="E23">
         <f t="shared" si="9"/>
         <v>254</v>
       </c>
-      <c r="F22">
+      <c r="F23">
         <f t="shared" si="9"/>
         <v>138</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <f t="shared" si="9"/>
         <v>136</v>
       </c>
-      <c r="H22">
+      <c r="H23">
         <f t="shared" si="9"/>
         <v>136</v>
       </c>
-      <c r="I22">
+      <c r="I23">
         <f t="shared" si="9"/>
         <v>136</v>
       </c>
-      <c r="J22">
+      <c r="J23">
         <f t="shared" si="9"/>
         <v>738</v>
       </c>
-      <c r="L22">
+      <c r="L23">
         <v>20799</v>
       </c>
-      <c r="M22">
+      <c r="M23">
         <v>73902</v>
       </c>
-      <c r="N22">
+      <c r="N23">
         <v>148346</v>
       </c>
-      <c r="O22">
+      <c r="O23">
         <v>8078</v>
       </c>
-      <c r="P22">
+      <c r="P23">
         <v>8754</v>
       </c>
-      <c r="Q22">
+      <c r="Q23">
         <v>136</v>
       </c>
-      <c r="R22">
-        <v>1</v>
-      </c>
-      <c r="S22">
+      <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="S23">
         <v>399177</v>
       </c>
-      <c r="U22">
+      <c r="U23">
         <v>-0.4500318872147781</v>
       </c>
-      <c r="V22">
+      <c r="V23">
         <v>-3.7188291265925137E-4</v>
       </c>
-      <c r="W22">
+      <c r="W23">
         <v>0.45011255844121684</v>
       </c>
-      <c r="X22">
+      <c r="X23">
         <v>7.484081655864177E-5</v>
       </c>
-      <c r="Y22">
+      <c r="Y23">
         <v>-7.3850145067154652E-5</v>
       </c>
-      <c r="Z22">
+      <c r="Z23">
         <v>5.1588013381318136E-5</v>
       </c>
-      <c r="AA22">
+      <c r="AA23">
         <v>2.3863300134775947E-4</v>
       </c>
-      <c r="AB22">
+      <c r="AB23">
         <v>2.4434950113864318E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>125</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <v>2863</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-      <c r="J23">
-        <v>1</v>
-      </c>
-      <c r="L23">
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="L24">
         <v>10313</v>
       </c>
-      <c r="M23">
+      <c r="M24">
         <v>43040</v>
       </c>
-      <c r="N23">
+      <c r="N24">
         <v>70238</v>
       </c>
-      <c r="O23">
+      <c r="O24">
         <v>12096</v>
       </c>
-      <c r="P23">
+      <c r="P24">
         <v>11754</v>
       </c>
-      <c r="Q23">
+      <c r="Q24">
         <v>738</v>
       </c>
-      <c r="R23">
-        <v>1</v>
-      </c>
-      <c r="S23">
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="S24">
         <v>210219</v>
       </c>
-      <c r="U23">
+      <c r="U24">
         <v>6.4998922410006674</v>
       </c>
-      <c r="V23">
+      <c r="V24">
         <v>-0.99222656328635406</v>
       </c>
-      <c r="W23">
+      <c r="W24">
         <v>-3.7371942565618377</v>
       </c>
-      <c r="X23">
+      <c r="X24">
         <v>-0.50196877306807286</v>
       </c>
-      <c r="Y23">
+      <c r="Y24">
         <v>2.2419439134118537E-3</v>
       </c>
-      <c r="Z23">
+      <c r="Z24">
         <v>-0.2517364906372061</v>
       </c>
-      <c r="AA23">
+      <c r="AA24">
         <v>-1.9008101360608636E-2</v>
       </c>
-      <c r="AB23">
+      <c r="AB24">
         <v>65.95965508962945</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>96</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>97</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L26" t="s">
         <v>128</v>
       </c>
-      <c r="P25" t="s">
+      <c r="P26" t="s">
         <v>132</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="Q26" t="s">
         <v>120</v>
       </c>
-      <c r="U25" t="s">
+      <c r="U26" t="s">
         <v>122</v>
       </c>
-      <c r="Y25" t="s">
+      <c r="Y26" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
         <v>88</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <v>9967</v>
       </c>
-      <c r="D26">
+      <c r="D27">
         <v>4</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <v>4</v>
       </c>
-      <c r="F26">
+      <c r="F27">
         <v>4</v>
       </c>
-      <c r="G26">
+      <c r="G27">
         <v>4</v>
       </c>
-      <c r="H26">
+      <c r="H27">
         <v>4</v>
       </c>
-      <c r="I26">
+      <c r="I27">
         <v>4</v>
       </c>
-      <c r="J26">
+      <c r="J27">
         <v>204</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K27" t="s">
         <v>129</v>
       </c>
-      <c r="L26">
-        <f>D17</f>
+      <c r="L27">
+        <f>D18</f>
         <v>7111</v>
       </c>
-      <c r="M26">
-        <f>E17</f>
+      <c r="M27">
+        <f>E18</f>
         <v>10767</v>
       </c>
-      <c r="N26">
-        <f>G17</f>
+      <c r="N27">
+        <f>G18</f>
         <v>7111</v>
       </c>
-      <c r="O26">
-        <f>J17</f>
+      <c r="O27">
+        <f>J18</f>
         <v>10313</v>
       </c>
-      <c r="P26">
-        <f>D4-D18-D21-D22</f>
+      <c r="P27">
+        <f>D4-D19-D22-D23</f>
         <v>138439</v>
       </c>
-      <c r="Q26" cm="1">
-        <f t="array" ref="Q26:T29">TRANSPOSE(L26:O29)</f>
+      <c r="Q27" cm="1">
+        <f t="array" ref="Q27:T30">TRANSPOSE(L27:O30)</f>
         <v>7111</v>
       </c>
-      <c r="R26">
+      <c r="R27">
         <v>66218</v>
       </c>
-      <c r="S26">
+      <c r="S27">
         <v>8076</v>
       </c>
-      <c r="T26">
-        <v>1</v>
-      </c>
-      <c r="U26" cm="1">
-        <f t="array" ref="U26:X29">MINVERSE(_xlfn.ANCHORARRAY(Q26))</f>
+      <c r="T27">
+        <v>1</v>
+      </c>
+      <c r="U27" cm="1">
+        <f t="array" ref="U27:X30">MINVERSE(_xlfn.ANCHORARRAY(Q27))</f>
         <v>-1.459775187242437E-4</v>
       </c>
-      <c r="V26">
+      <c r="V27">
         <v>6.4553709512161193E-4</v>
       </c>
-      <c r="W26">
+      <c r="W27">
         <v>-7.4798920630780795E-5</v>
       </c>
-      <c r="X26">
+      <c r="X27">
         <v>-4.247606557665874E-4</v>
       </c>
-      <c r="Y26" cm="1">
-        <f t="array" ref="Y26:Y29">MMULT(_xlfn.ANCHORARRAY(U26),P26:P29)</f>
+      <c r="Y27" cm="1">
+        <f t="array" ref="Y27:Y30">MMULT(_xlfn.ANCHORARRAY(U27),P27:P30)</f>
         <v>5.0512537183762731</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
         <v>89</v>
       </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-      <c r="I27">
-        <v>1</v>
-      </c>
-      <c r="J27">
-        <v>1</v>
-      </c>
-      <c r="K27" t="s">
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28" t="s">
         <v>130</v>
-      </c>
-      <c r="L27">
-        <f>D19</f>
-        <v>66218</v>
-      </c>
-      <c r="M27">
-        <f>E19</f>
-        <v>76950</v>
-      </c>
-      <c r="N27">
-        <f>G19</f>
-        <v>136010</v>
-      </c>
-      <c r="O27">
-        <f>J19</f>
-        <v>70238</v>
-      </c>
-      <c r="P27">
-        <f>E4-E18-E21-E22</f>
-        <v>171107</v>
-      </c>
-      <c r="Q27">
-        <v>10767</v>
-      </c>
-      <c r="R27">
-        <v>76950</v>
-      </c>
-      <c r="S27">
-        <v>11732</v>
-      </c>
-      <c r="T27">
-        <v>1</v>
-      </c>
-      <c r="U27">
-        <v>2.550895020265855E-6</v>
-      </c>
-      <c r="V27">
-        <v>7.3454505280007157E-5</v>
-      </c>
-      <c r="W27">
-        <v>7.8639536359250295E-6</v>
-      </c>
-      <c r="X27">
-        <v>-8.3869353936198078E-5</v>
-      </c>
-      <c r="Y27">
-        <v>1.9973743570092619</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28">
-        <v>63</v>
-      </c>
-      <c r="D28">
-        <v>128</v>
-      </c>
-      <c r="E28">
-        <v>246</v>
-      </c>
-      <c r="F28">
-        <v>130</v>
-      </c>
-      <c r="G28">
-        <v>128</v>
-      </c>
-      <c r="H28">
-        <v>128</v>
-      </c>
-      <c r="I28">
-        <v>128</v>
-      </c>
-      <c r="J28">
-        <v>530</v>
-      </c>
-      <c r="K28" t="s">
-        <v>131</v>
       </c>
       <c r="L28">
         <f>D20</f>
-        <v>8076</v>
+        <v>66218</v>
       </c>
       <c r="M28">
         <f>E20</f>
-        <v>11732</v>
+        <v>76950</v>
       </c>
       <c r="N28">
         <f>G20</f>
-        <v>16800</v>
+        <v>136010</v>
       </c>
       <c r="O28">
         <f>J20</f>
+        <v>70238</v>
+      </c>
+      <c r="P28">
+        <f>E4-E19-E22-E23</f>
+        <v>171107</v>
+      </c>
+      <c r="Q28">
+        <v>10767</v>
+      </c>
+      <c r="R28">
+        <v>76950</v>
+      </c>
+      <c r="S28">
+        <v>11732</v>
+      </c>
+      <c r="T28">
+        <v>1</v>
+      </c>
+      <c r="U28">
+        <v>2.550895020265855E-6</v>
+      </c>
+      <c r="V28">
+        <v>7.3454505280007157E-5</v>
+      </c>
+      <c r="W28">
+        <v>7.8639536359250295E-6</v>
+      </c>
+      <c r="X28">
+        <v>-8.3869353936198078E-5</v>
+      </c>
+      <c r="Y28">
+        <v>1.9973743570092619</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29">
+        <v>63</v>
+      </c>
+      <c r="D29">
+        <v>128</v>
+      </c>
+      <c r="E29">
+        <v>246</v>
+      </c>
+      <c r="F29">
+        <v>130</v>
+      </c>
+      <c r="G29">
+        <v>128</v>
+      </c>
+      <c r="H29">
+        <v>128</v>
+      </c>
+      <c r="I29">
+        <v>128</v>
+      </c>
+      <c r="J29">
+        <v>530</v>
+      </c>
+      <c r="K29" t="s">
+        <v>131</v>
+      </c>
+      <c r="L29">
+        <f>D21</f>
+        <v>8076</v>
+      </c>
+      <c r="M29">
+        <f>E21</f>
+        <v>11732</v>
+      </c>
+      <c r="N29">
+        <f>G21</f>
+        <v>16800</v>
+      </c>
+      <c r="O29">
+        <f>J21</f>
         <v>12096</v>
       </c>
-      <c r="P28">
-        <f>G4-G18-G21-G22</f>
+      <c r="P29">
+        <f>G4-G19-G22-G23</f>
         <v>260575</v>
       </c>
-      <c r="Q28">
+      <c r="Q29">
         <v>7111</v>
       </c>
-      <c r="R28">
+      <c r="R29">
         <v>136010</v>
       </c>
-      <c r="S28">
+      <c r="S29">
         <v>16800</v>
       </c>
-      <c r="T28">
-        <v>1</v>
-      </c>
-      <c r="U28">
+      <c r="T29">
+        <v>1</v>
+      </c>
+      <c r="U29">
         <v>-1.3503347836478616E-4</v>
       </c>
-      <c r="V28">
+      <c r="V29">
         <v>-5.8763604224005726E-4</v>
       </c>
-      <c r="W28">
+      <c r="W29">
         <v>5.1714689115259085E-5</v>
       </c>
-      <c r="X28">
+      <c r="X29">
         <v>6.7095483148958452E-4</v>
       </c>
-      <c r="Y28">
+      <c r="Y29">
         <v>-1.9789948560741237</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>67</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29">
-        <v>6</v>
-      </c>
-      <c r="E29">
-        <v>6</v>
-      </c>
-      <c r="F29">
-        <v>6</v>
-      </c>
-      <c r="G29">
-        <v>6</v>
-      </c>
-      <c r="H29">
-        <v>6</v>
-      </c>
-      <c r="I29">
-        <v>6</v>
-      </c>
-      <c r="J29">
-        <v>206</v>
-      </c>
-      <c r="K29" t="s">
-        <v>125</v>
-      </c>
-      <c r="L29">
-        <v>1</v>
-      </c>
-      <c r="M29">
-        <v>1</v>
-      </c>
-      <c r="N29">
-        <v>1</v>
-      </c>
-      <c r="O29">
-        <v>1</v>
-      </c>
-      <c r="P29">
-        <f>J4-J18-J21-J22</f>
-        <v>154687</v>
-      </c>
-      <c r="Q29">
-        <v>10313</v>
-      </c>
-      <c r="R29">
-        <v>70238</v>
-      </c>
-      <c r="S29">
-        <v>12096</v>
-      </c>
-      <c r="T29">
-        <v>1</v>
-      </c>
-      <c r="U29">
-        <v>2.9596613404701455</v>
-      </c>
-      <c r="V29">
-        <v>-4.7086760369105942</v>
-      </c>
-      <c r="W29">
-        <v>-0.4064879865530337</v>
-      </c>
-      <c r="X29">
-        <v>3.1555026829934829</v>
-      </c>
-      <c r="Y29">
-        <v>-13760.237906158436</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" t="s">
-        <v>68</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
       <c r="D30">
+        <v>6</v>
+      </c>
+      <c r="E30">
+        <v>6</v>
+      </c>
+      <c r="F30">
+        <v>6</v>
+      </c>
+      <c r="G30">
+        <v>6</v>
+      </c>
+      <c r="H30">
+        <v>6</v>
+      </c>
+      <c r="I30">
+        <v>6</v>
+      </c>
+      <c r="J30">
+        <v>206</v>
+      </c>
+      <c r="K30" t="s">
+        <v>125</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30">
+        <v>1</v>
+      </c>
+      <c r="P30">
+        <f>J4-J19-J22-J23</f>
+        <v>154687</v>
+      </c>
+      <c r="Q30">
+        <v>10313</v>
+      </c>
+      <c r="R30">
+        <v>70238</v>
+      </c>
+      <c r="S30">
+        <v>12096</v>
+      </c>
+      <c r="T30">
+        <v>1</v>
+      </c>
+      <c r="U30">
+        <v>2.9596613404701455</v>
+      </c>
+      <c r="V30">
+        <v>-4.7086760369105942</v>
+      </c>
+      <c r="W30">
+        <v>-0.4064879865530337</v>
+      </c>
+      <c r="X30">
+        <v>3.1555026829934829</v>
+      </c>
+      <c r="Y30">
+        <v>-13760.237906158436</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31">
         <v>2</v>
       </c>
-      <c r="E30">
+      <c r="D31">
         <v>2</v>
       </c>
-      <c r="F30">
+      <c r="E31">
         <v>2</v>
       </c>
-      <c r="G30">
+      <c r="F31">
         <v>2</v>
       </c>
-      <c r="H30">
+      <c r="G31">
         <v>2</v>
       </c>
-      <c r="I30">
+      <c r="H31">
         <v>2</v>
       </c>
-      <c r="J30">
+      <c r="I31">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="J31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>69</v>
       </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
         <v>4</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <v>4</v>
       </c>
-      <c r="F31">
+      <c r="F32">
         <v>4</v>
       </c>
-      <c r="G31">
+      <c r="G32">
         <v>4</v>
       </c>
-      <c r="H31">
+      <c r="H32">
         <v>4</v>
       </c>
-      <c r="I31">
+      <c r="I32">
         <v>4</v>
       </c>
-      <c r="J31">
+      <c r="J32">
         <v>404</v>
       </c>
-      <c r="L31" t="s">
+      <c r="L32" t="s">
         <v>128</v>
       </c>
-      <c r="P31" t="s">
+      <c r="P32" t="s">
         <v>132</v>
       </c>
-      <c r="R31" t="s">
+      <c r="R32" t="s">
         <v>120</v>
       </c>
-      <c r="U31" t="s">
+      <c r="U32" t="s">
         <v>122</v>
       </c>
-      <c r="Y31" t="s">
+      <c r="Y32" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>70</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <v>1829</v>
       </c>
-      <c r="D32">
+      <c r="D33">
         <v>3657</v>
       </c>
-      <c r="E32">
+      <c r="E33">
         <v>7313</v>
       </c>
-      <c r="F32">
+      <c r="F33">
         <v>3659</v>
       </c>
-      <c r="G32">
+      <c r="G33">
         <v>3657</v>
       </c>
-      <c r="H32">
+      <c r="H33">
         <v>3657</v>
       </c>
-      <c r="I32">
+      <c r="I33">
         <v>3657</v>
       </c>
-      <c r="J32">
+      <c r="J33">
         <v>3657</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K33" t="s">
         <v>129</v>
       </c>
-      <c r="L32">
-        <f>D17</f>
+      <c r="L33">
+        <f>D18</f>
         <v>7111</v>
       </c>
-      <c r="M32">
-        <f>E17</f>
+      <c r="M33">
+        <f>E18</f>
         <v>10767</v>
       </c>
-      <c r="N32">
-        <f>G17</f>
+      <c r="N33">
+        <f>G18</f>
         <v>7111</v>
       </c>
-      <c r="P32">
-        <f>D4-D18-D21-D22</f>
+      <c r="P33">
+        <f>D4-D19-D22-D23</f>
         <v>138439</v>
       </c>
-      <c r="R32" cm="1">
-        <f t="array" ref="R32:T34">TRANSPOSE(L32:N34)</f>
+      <c r="R33" cm="1">
+        <f t="array" ref="R33:T35">TRANSPOSE(L33:N35)</f>
         <v>7111</v>
       </c>
-      <c r="S32">
+      <c r="S33">
         <v>74294</v>
       </c>
-      <c r="T32">
-        <v>1</v>
-      </c>
-      <c r="U32" cm="1">
-        <f t="array" ref="U32:W34">MINVERSE(_xlfn.ANCHORARRAY(R32))</f>
+      <c r="T33">
+        <v>1</v>
+      </c>
+      <c r="U33" cm="1">
+        <f t="array" ref="U33:W35">MINVERSE(_xlfn.ANCHORARRAY(R33))</f>
         <v>-2.2340008915937691E-4</v>
       </c>
-      <c r="V32">
+      <c r="V33">
         <v>2.7352297592997811E-4</v>
       </c>
-      <c r="W32">
+      <c r="W33">
         <v>-5.0122886770601223E-5</v>
       </c>
-      <c r="Y32" cm="1">
-        <f t="array" ref="Y32:Y34">MMULT(_xlfn.ANCHORARRAY(U32),P32:P34)</f>
+      <c r="Y33" cm="1">
+        <f t="array" ref="Y33:Y35">MMULT(_xlfn.ANCHORARRAY(U33),P33:P35)</f>
         <v>2.813639679066366</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>71</v>
       </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-      <c r="J33">
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
         <v>202</v>
       </c>
-      <c r="K33" t="s">
+      <c r="K34" t="s">
         <v>134</v>
       </c>
-      <c r="L33">
-        <f>L27+L28</f>
+      <c r="L34">
+        <f>L28+L29</f>
         <v>74294</v>
       </c>
-      <c r="M33">
-        <f t="shared" ref="M33:N33" si="10">M27+M28</f>
+      <c r="M34">
+        <f t="shared" ref="M34:N34" si="10">M28+M29</f>
         <v>88682</v>
       </c>
-      <c r="N33">
+      <c r="N34">
         <f t="shared" si="10"/>
         <v>152810</v>
       </c>
-      <c r="P33">
-        <f>E4-E18-E21-E22</f>
+      <c r="P34">
+        <f>E4-E19-E22-E23</f>
         <v>171107</v>
       </c>
-      <c r="R33">
+      <c r="R34">
         <v>10767</v>
       </c>
-      <c r="S33">
+      <c r="S34">
         <v>88682</v>
       </c>
-      <c r="T33">
-        <v>1</v>
-      </c>
-      <c r="U33">
+      <c r="T34">
+        <v>1</v>
+      </c>
+      <c r="U34">
         <v>-1.2736257578073259E-5</v>
       </c>
-      <c r="V33">
-        <v>0</v>
-      </c>
-      <c r="W33">
+      <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="W34">
         <v>1.2736257578073259E-5</v>
       </c>
-      <c r="Y33">
+      <c r="Y34">
         <v>1.5555555555555556</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>72</v>
       </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
         <v>22</v>
       </c>
-      <c r="E34">
+      <c r="E35">
         <v>22</v>
       </c>
-      <c r="F34">
+      <c r="F35">
         <v>22</v>
       </c>
-      <c r="G34">
+      <c r="G35">
         <v>22</v>
       </c>
-      <c r="H34">
+      <c r="H35">
         <v>22</v>
       </c>
-      <c r="I34">
+      <c r="I35">
         <v>22</v>
       </c>
-      <c r="J34">
+      <c r="J35">
         <v>2222</v>
       </c>
-      <c r="K34" t="s">
+      <c r="K35" t="s">
         <v>125</v>
       </c>
-      <c r="L34">
-        <v>1</v>
-      </c>
-      <c r="M34">
-        <v>1</v>
-      </c>
-      <c r="N34">
-        <v>1</v>
-      </c>
-      <c r="P34">
-        <f>G4-G18-G21-G22</f>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="P35">
+        <f>G4-G19-G22-G23</f>
         <v>260575</v>
       </c>
-      <c r="R34">
+      <c r="R35">
         <v>7111</v>
       </c>
-      <c r="S34">
+      <c r="S35">
         <v>152810</v>
       </c>
-      <c r="T34">
-        <v>1</v>
-      </c>
-      <c r="U34">
+      <c r="T35">
+        <v>1</v>
+      </c>
+      <c r="U35">
         <v>3.5348255545177039</v>
       </c>
-      <c r="V34">
+      <c r="V35">
         <v>-1.9450218818380745</v>
       </c>
-      <c r="W34">
+      <c r="W35">
         <v>-0.58980367267962941</v>
       </c>
-      <c r="Y34">
+      <c r="Y35">
         <v>2862.7637977146078</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>73</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <v>1711</v>
       </c>
-      <c r="D35">
+      <c r="D36">
         <v>3426</v>
       </c>
-      <c r="E35">
+      <c r="E36">
         <v>3426</v>
       </c>
-      <c r="F35">
+      <c r="F36">
         <v>3426</v>
       </c>
-      <c r="G35">
+      <c r="G36">
         <v>3426</v>
       </c>
-      <c r="H35">
+      <c r="H36">
         <v>17114</v>
       </c>
-      <c r="I35">
+      <c r="I36">
         <v>17114</v>
       </c>
-      <c r="J35">
+      <c r="J36">
         <v>3826</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>83</v>
       </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>84</v>
       </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>80</v>
       </c>
-      <c r="C38">
+      <c r="C39">
         <v>15346</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <v>50644</v>
       </c>
-      <c r="E38">
+      <c r="E39">
         <v>61376</v>
       </c>
-      <c r="F38">
+      <c r="F39">
         <v>50646</v>
       </c>
-      <c r="G38">
+      <c r="G39">
         <v>102988</v>
       </c>
-      <c r="H38">
+      <c r="H39">
         <v>122504</v>
       </c>
-      <c r="I38">
+      <c r="I39">
         <v>105396</v>
       </c>
-      <c r="J38">
+      <c r="J39">
         <v>54064</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>82</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <v>7784</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <v>15574</v>
       </c>
-      <c r="E39">
+      <c r="E40">
         <v>15574</v>
       </c>
-      <c r="F39">
+      <c r="F40">
         <v>15574</v>
       </c>
-      <c r="G39">
+      <c r="G40">
         <v>33022</v>
       </c>
-      <c r="H39">
+      <c r="H40">
         <v>42950</v>
       </c>
-      <c r="I39">
+      <c r="I40">
         <v>42950</v>
       </c>
-      <c r="J39">
+      <c r="J40">
         <v>16174</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>81</v>
       </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>85</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <v>2181</v>
       </c>
-      <c r="D41">
+      <c r="D42">
         <v>4368</v>
       </c>
-      <c r="E41">
+      <c r="E42">
         <v>4368</v>
       </c>
-      <c r="F41">
+      <c r="F42">
         <v>4368</v>
       </c>
-      <c r="G41">
+      <c r="G42">
         <v>13092</v>
       </c>
-      <c r="H41">
+      <c r="H42">
         <v>4368</v>
       </c>
-      <c r="I41">
+      <c r="I42">
         <v>4368</v>
       </c>
-      <c r="J41">
+      <c r="J42">
         <v>4968</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>87</v>
       </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-      <c r="J42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>86</v>
       </c>
-      <c r="C43">
+      <c r="C44">
         <v>1841</v>
       </c>
-      <c r="D43">
+      <c r="D44">
         <v>3708</v>
       </c>
-      <c r="E43">
+      <c r="E44">
         <v>7364</v>
       </c>
-      <c r="F43">
+      <c r="F44">
         <v>3708</v>
       </c>
-      <c r="G43">
+      <c r="G44">
         <v>3708</v>
       </c>
-      <c r="H43">
+      <c r="H44">
         <v>7130</v>
       </c>
-      <c r="I43">
+      <c r="I44">
         <v>3710</v>
       </c>
-      <c r="J43">
+      <c r="J44">
         <v>7128</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>78</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <v>16375</v>
       </c>
-      <c r="D44">
+      <c r="D45">
         <v>12898</v>
       </c>
-      <c r="E44">
+      <c r="E45">
         <v>16440</v>
       </c>
-      <c r="F44">
+      <c r="F45">
         <v>12898</v>
       </c>
-      <c r="G44">
+      <c r="G45">
         <v>24530</v>
       </c>
-      <c r="H44">
+      <c r="H45">
         <v>36850</v>
       </c>
-      <c r="I44">
+      <c r="I45">
         <v>26586</v>
       </c>
-      <c r="J44">
+      <c r="J45">
         <v>22100</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>19</v>
       </c>
-      <c r="C45">
-        <v>0</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-      <c r="J45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>20</v>
       </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-      <c r="I46">
-        <v>0</v>
-      </c>
-      <c r="J46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>21</v>
       </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
-      <c r="I47">
-        <v>0</v>
-      </c>
-      <c r="J47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>22</v>
       </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-      <c r="I48">
-        <v>0</v>
-      </c>
-      <c r="J48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>79</v>
       </c>
-      <c r="C49">
+      <c r="C50">
         <v>2181</v>
       </c>
-      <c r="D49">
+      <c r="D50">
         <v>4370</v>
       </c>
-      <c r="E49">
+      <c r="E50">
         <v>4370</v>
       </c>
-      <c r="F49">
+      <c r="F50">
         <v>4370</v>
       </c>
-      <c r="G49">
+      <c r="G50">
         <v>13094</v>
       </c>
-      <c r="H49">
+      <c r="H50">
         <v>4370</v>
       </c>
-      <c r="I49">
+      <c r="I50">
         <v>4370</v>
       </c>
-      <c r="J49">
+      <c r="J50">
         <v>5170</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B50" t="s">
-        <v>119</v>
-      </c>
-      <c r="C50">
-        <v>0</v>
-      </c>
-      <c r="D50">
-        <v>10</v>
-      </c>
-      <c r="E50">
-        <v>10</v>
-      </c>
-      <c r="F50">
-        <v>10</v>
-      </c>
-      <c r="G50">
-        <v>10</v>
-      </c>
-      <c r="H50">
-        <v>10</v>
-      </c>
-      <c r="I50">
-        <v>10</v>
-      </c>
-      <c r="J50">
-        <v>1010</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="B51" t="s">
         <v>119</v>
@@ -3466,30 +3466,30 @@
         <v>0</v>
       </c>
       <c r="D51">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E51">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F51">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G51">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H51">
-        <v>13694</v>
+        <v>10</v>
       </c>
       <c r="I51">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J51">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B52" t="s">
         <v>119</v>
@@ -3498,878 +3498,910 @@
         <v>0</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H52">
+        <v>13694</v>
+      </c>
+      <c r="I52">
+        <v>6</v>
+      </c>
+      <c r="J52">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" t="s">
+        <v>119</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
         <v>13688</v>
       </c>
-      <c r="I52">
-        <v>0</v>
-      </c>
-      <c r="J52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>56</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <v>9965</v>
       </c>
-      <c r="D53">
+      <c r="D54">
         <v>19936</v>
       </c>
-      <c r="E53">
+      <c r="E54">
         <v>19936</v>
       </c>
-      <c r="F53">
+      <c r="F54">
         <v>19936</v>
       </c>
-      <c r="G53">
+      <c r="G54">
         <v>46108</v>
       </c>
-      <c r="H53">
+      <c r="H54">
         <v>64422</v>
       </c>
-      <c r="I53">
+      <c r="I54">
         <v>47312</v>
       </c>
-      <c r="J53">
+      <c r="J54">
         <v>20536</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>57</v>
       </c>
-      <c r="C54">
-        <v>0</v>
-      </c>
-      <c r="D54">
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
         <v>4</v>
       </c>
-      <c r="E54">
+      <c r="E55">
         <v>4</v>
       </c>
-      <c r="F54">
+      <c r="F55">
         <v>4</v>
       </c>
-      <c r="G54">
+      <c r="G55">
         <v>4</v>
       </c>
-      <c r="H54">
+      <c r="H55">
         <v>13692</v>
       </c>
-      <c r="I54">
+      <c r="I55">
         <v>4</v>
       </c>
-      <c r="J54">
+      <c r="J55">
         <v>404</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>65</v>
       </c>
-      <c r="C55">
-        <v>0</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-      <c r="F55">
-        <v>0</v>
-      </c>
-      <c r="G55">
-        <v>0</v>
-      </c>
-      <c r="H55">
-        <v>0</v>
-      </c>
-      <c r="I55">
-        <v>0</v>
-      </c>
-      <c r="J55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>58</v>
       </c>
-      <c r="C56">
-        <v>0</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-      <c r="F56">
-        <v>0</v>
-      </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56">
-        <v>0</v>
-      </c>
-      <c r="J56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>59</v>
       </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57">
-        <v>0</v>
-      </c>
-      <c r="F57">
-        <v>0</v>
-      </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-      <c r="H57">
-        <v>0</v>
-      </c>
-      <c r="I57">
-        <v>0</v>
-      </c>
-      <c r="J57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>60</v>
       </c>
-      <c r="C58">
+      <c r="C59">
         <v>2181</v>
       </c>
-      <c r="D58">
+      <c r="D59">
         <v>4364</v>
       </c>
-      <c r="E58">
+      <c r="E59">
         <v>4364</v>
       </c>
-      <c r="F58">
+      <c r="F59">
         <v>4364</v>
       </c>
-      <c r="G58">
+      <c r="G59">
         <v>13088</v>
       </c>
-      <c r="H58">
+      <c r="H59">
         <v>4364</v>
       </c>
-      <c r="I58">
+      <c r="I59">
         <v>4364</v>
       </c>
-      <c r="J58">
+      <c r="J59">
         <v>4564</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>63</v>
       </c>
-      <c r="C59">
-        <v>0</v>
-      </c>
-      <c r="D59">
-        <v>0</v>
-      </c>
-      <c r="E59">
-        <v>0</v>
-      </c>
-      <c r="F59">
-        <v>0</v>
-      </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-      <c r="I59">
-        <v>0</v>
-      </c>
-      <c r="J59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>64</v>
       </c>
-      <c r="C60">
-        <v>0</v>
-      </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
-      <c r="E60">
-        <v>0</v>
-      </c>
-      <c r="F60">
-        <v>0</v>
-      </c>
-      <c r="G60">
-        <v>0</v>
-      </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
-      <c r="I60">
-        <v>0</v>
-      </c>
-      <c r="J60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>61</v>
       </c>
-      <c r="C61">
-        <v>0</v>
-      </c>
-      <c r="D61">
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
         <v>4</v>
       </c>
-      <c r="E61">
+      <c r="E62">
         <v>4</v>
       </c>
-      <c r="F61">
+      <c r="F62">
         <v>4</v>
       </c>
-      <c r="G61">
+      <c r="G62">
         <v>4</v>
       </c>
-      <c r="H61">
+      <c r="H62">
         <v>4</v>
       </c>
-      <c r="I61">
+      <c r="I62">
         <v>4</v>
       </c>
-      <c r="J61">
+      <c r="J62">
         <v>404</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>62</v>
       </c>
-      <c r="C62">
-        <v>0</v>
-      </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-      <c r="F62">
-        <v>0</v>
-      </c>
-      <c r="G62">
-        <v>0</v>
-      </c>
-      <c r="H62">
-        <v>0</v>
-      </c>
-      <c r="I62">
-        <v>0</v>
-      </c>
-      <c r="J62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>75</v>
       </c>
-      <c r="C63">
-        <v>0</v>
-      </c>
-      <c r="D63">
-        <v>0</v>
-      </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-      <c r="F63">
-        <v>0</v>
-      </c>
-      <c r="G63">
-        <v>0</v>
-      </c>
-      <c r="H63">
-        <v>0</v>
-      </c>
-      <c r="I63">
-        <v>0</v>
-      </c>
-      <c r="J63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>74</v>
       </c>
-      <c r="C64">
-        <v>0</v>
-      </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-      <c r="E64">
-        <v>0</v>
-      </c>
-      <c r="F64">
-        <v>0</v>
-      </c>
-      <c r="G64">
-        <v>0</v>
-      </c>
-      <c r="H64">
-        <v>0</v>
-      </c>
-      <c r="I64">
-        <v>0</v>
-      </c>
-      <c r="J64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>76</v>
       </c>
-      <c r="C65">
-        <v>1</v>
-      </c>
-      <c r="D65">
-        <v>1</v>
-      </c>
-      <c r="E65">
-        <v>1</v>
-      </c>
-      <c r="F65">
-        <v>1</v>
-      </c>
-      <c r="G65">
-        <v>1</v>
-      </c>
-      <c r="H65">
-        <v>1</v>
-      </c>
-      <c r="I65">
-        <v>1</v>
-      </c>
-      <c r="J65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>77</v>
       </c>
-      <c r="C66">
-        <v>0</v>
-      </c>
-      <c r="D66">
-        <v>0</v>
-      </c>
-      <c r="E66">
-        <v>0</v>
-      </c>
-      <c r="F66">
-        <v>0</v>
-      </c>
-      <c r="G66">
-        <v>0</v>
-      </c>
-      <c r="H66">
-        <v>0</v>
-      </c>
-      <c r="I66">
-        <v>0</v>
-      </c>
-      <c r="J66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>41</v>
       </c>
-      <c r="C67">
-        <v>0</v>
-      </c>
-      <c r="D67">
-        <v>0</v>
-      </c>
-      <c r="E67">
-        <v>0</v>
-      </c>
-      <c r="F67">
-        <v>0</v>
-      </c>
-      <c r="G67">
-        <v>0</v>
-      </c>
-      <c r="H67">
-        <v>0</v>
-      </c>
-      <c r="I67">
-        <v>0</v>
-      </c>
-      <c r="J67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>42</v>
       </c>
-      <c r="C68">
-        <v>0</v>
-      </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-      <c r="F68">
-        <v>0</v>
-      </c>
-      <c r="G68">
-        <v>0</v>
-      </c>
-      <c r="H68">
-        <v>0</v>
-      </c>
-      <c r="I68">
-        <v>0</v>
-      </c>
-      <c r="J68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>43</v>
       </c>
-      <c r="C69">
-        <v>0</v>
-      </c>
-      <c r="D69">
-        <v>0</v>
-      </c>
-      <c r="E69">
-        <v>0</v>
-      </c>
-      <c r="F69">
-        <v>0</v>
-      </c>
-      <c r="G69">
-        <v>0</v>
-      </c>
-      <c r="H69">
-        <v>0</v>
-      </c>
-      <c r="I69">
-        <v>0</v>
-      </c>
-      <c r="J69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>44</v>
       </c>
-      <c r="C70">
-        <v>0</v>
-      </c>
-      <c r="D70">
-        <v>0</v>
-      </c>
-      <c r="E70">
-        <v>0</v>
-      </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
-      <c r="G70">
-        <v>0</v>
-      </c>
-      <c r="H70">
-        <v>0</v>
-      </c>
-      <c r="I70">
-        <v>0</v>
-      </c>
-      <c r="J70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>45</v>
       </c>
-      <c r="C71">
-        <v>0</v>
-      </c>
-      <c r="D71">
-        <v>0</v>
-      </c>
-      <c r="E71">
-        <v>0</v>
-      </c>
-      <c r="F71">
-        <v>0</v>
-      </c>
-      <c r="G71">
-        <v>0</v>
-      </c>
-      <c r="H71">
-        <v>0</v>
-      </c>
-      <c r="I71">
-        <v>0</v>
-      </c>
-      <c r="J71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>46</v>
       </c>
-      <c r="C72">
-        <v>0</v>
-      </c>
-      <c r="D72">
-        <v>0</v>
-      </c>
-      <c r="E72">
-        <v>0</v>
-      </c>
-      <c r="F72">
-        <v>0</v>
-      </c>
-      <c r="G72">
-        <v>0</v>
-      </c>
-      <c r="H72">
-        <v>0</v>
-      </c>
-      <c r="I72">
-        <v>0</v>
-      </c>
-      <c r="J72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>47</v>
       </c>
-      <c r="C73">
-        <v>0</v>
-      </c>
-      <c r="D73">
-        <v>0</v>
-      </c>
-      <c r="E73">
-        <v>0</v>
-      </c>
-      <c r="F73">
-        <v>0</v>
-      </c>
-      <c r="G73">
-        <v>0</v>
-      </c>
-      <c r="H73">
-        <v>0</v>
-      </c>
-      <c r="I73">
-        <v>0</v>
-      </c>
-      <c r="J73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>48</v>
       </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-      <c r="D74">
-        <v>0</v>
-      </c>
-      <c r="E74">
-        <v>0</v>
-      </c>
-      <c r="F74">
-        <v>0</v>
-      </c>
-      <c r="G74">
-        <v>0</v>
-      </c>
-      <c r="H74">
-        <v>0</v>
-      </c>
-      <c r="I74">
-        <v>0</v>
-      </c>
-      <c r="J74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>49</v>
       </c>
-      <c r="C75">
-        <v>0</v>
-      </c>
-      <c r="D75">
-        <v>0</v>
-      </c>
-      <c r="E75">
-        <v>0</v>
-      </c>
-      <c r="F75">
-        <v>0</v>
-      </c>
-      <c r="G75">
-        <v>0</v>
-      </c>
-      <c r="H75">
-        <v>0</v>
-      </c>
-      <c r="I75">
-        <v>0</v>
-      </c>
-      <c r="J75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>50</v>
       </c>
-      <c r="C76">
-        <v>0</v>
-      </c>
-      <c r="D76">
-        <v>0</v>
-      </c>
-      <c r="E76">
-        <v>0</v>
-      </c>
-      <c r="F76">
-        <v>0</v>
-      </c>
-      <c r="G76">
-        <v>0</v>
-      </c>
-      <c r="H76">
-        <v>0</v>
-      </c>
-      <c r="I76">
-        <v>0</v>
-      </c>
-      <c r="J76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>51</v>
       </c>
-      <c r="C77">
-        <v>0</v>
-      </c>
-      <c r="D77">
-        <v>0</v>
-      </c>
-      <c r="E77">
-        <v>0</v>
-      </c>
-      <c r="F77">
-        <v>0</v>
-      </c>
-      <c r="G77">
-        <v>0</v>
-      </c>
-      <c r="H77">
-        <v>0</v>
-      </c>
-      <c r="I77">
-        <v>0</v>
-      </c>
-      <c r="J77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>52</v>
       </c>
-      <c r="C78">
-        <v>0</v>
-      </c>
-      <c r="D78">
-        <v>0</v>
-      </c>
-      <c r="E78">
-        <v>0</v>
-      </c>
-      <c r="F78">
-        <v>0</v>
-      </c>
-      <c r="G78">
-        <v>0</v>
-      </c>
-      <c r="H78">
-        <v>0</v>
-      </c>
-      <c r="I78">
-        <v>0</v>
-      </c>
-      <c r="J78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>53</v>
       </c>
-      <c r="C79">
-        <v>0</v>
-      </c>
-      <c r="D79">
-        <v>0</v>
-      </c>
-      <c r="E79">
-        <v>0</v>
-      </c>
-      <c r="F79">
-        <v>0</v>
-      </c>
-      <c r="G79">
-        <v>0</v>
-      </c>
-      <c r="H79">
-        <v>0</v>
-      </c>
-      <c r="I79">
-        <v>0</v>
-      </c>
-      <c r="J79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>54</v>
       </c>
-      <c r="C80">
-        <v>0</v>
-      </c>
-      <c r="D80">
-        <v>0</v>
-      </c>
-      <c r="E80">
-        <v>0</v>
-      </c>
-      <c r="F80">
-        <v>0</v>
-      </c>
-      <c r="G80">
-        <v>0</v>
-      </c>
-      <c r="H80">
-        <v>0</v>
-      </c>
-      <c r="I80">
-        <v>0</v>
-      </c>
-      <c r="J80">
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+      <c r="J81">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correcting bsort alu verify
</commit_message>
<xml_diff>
--- a/verilog/hardware/processor/source/instruction_counts.xlsx
+++ b/verilog/hardware/processor/source/instruction_counts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcos/GB3/f-of-e-tools/verilog/hardware/processor/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02779258-6888-9F43-90CA-5C6676443BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09964BF3-ABAF-FF48-B47C-23B21695255D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1360" windowWidth="27000" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instruction_counts" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="145">
   <si>
     <t>LUI</t>
   </si>
@@ -485,6 +485,9 @@
   </si>
   <si>
     <t>Baseline Average Dynamic Power</t>
+  </si>
+  <si>
+    <t>Device Utilisation</t>
   </si>
 </sst>
 </file>
@@ -1335,10 +1338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC82"/>
+  <dimension ref="A1:AC83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1705,11 +1708,11 @@
         <v>142</v>
       </c>
       <c r="C13">
-        <f>100*SUM(C32:C37)/SUM(C28:C82)</f>
+        <f>100*SUM(C33:C38)/SUM(C29:C83)</f>
         <v>4.9587008259834802</v>
       </c>
       <c r="D13">
-        <f t="shared" ref="D13:K13" si="5">100*SUM(D32:D37)/SUM(D28:D82)</f>
+        <f t="shared" ref="D13:K13" si="5">100*SUM(D33:D38)/SUM(D29:D83)</f>
         <v>5.7748686422440043</v>
       </c>
       <c r="E13">
@@ -1741,1459 +1744,1429 @@
         <v>12.115294485236682</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>137</v>
       </c>
-      <c r="C15">
-        <f>(C4-C20*$B20-C21*$B21-C22*$B22-C23*$B23-C24*$B24-C25*$B25)/C19</f>
+      <c r="C16">
+        <f>(C4-C21*$B21-C22*$B22-C23*$B23-C24*$B24-C25*$B25-C26*$B26)/C20</f>
         <v>2.7175042348955398</v>
       </c>
-      <c r="D15">
-        <f t="shared" ref="D15:J15" si="6">(D4-D20*$B20-D21*$B21-D22*$B22-D23*$B23-D24*$B24-D25*$B25)/D19</f>
+      <c r="D16">
+        <f t="shared" ref="D16:J16" si="6">(D4-D21*$B21-D22*$B22-D23*$B23-D24*$B24-D25*$B25-D26*$B26)/D20</f>
         <v>2.8716495570243268</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <f t="shared" si="6"/>
         <v>2.8593758707160766</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <f t="shared" si="6"/>
         <v>2.8720933502038517</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <f t="shared" si="6"/>
         <v>2.9329911404865703</v>
       </c>
-      <c r="H15">
+      <c r="H16">
         <f t="shared" si="6"/>
         <v>4.0255012260204817</v>
       </c>
-      <c r="I15">
+      <c r="I16">
         <f t="shared" si="6"/>
         <v>3.4167411894802631</v>
       </c>
-      <c r="J15">
+      <c r="J16">
         <f t="shared" si="6"/>
         <v>2.3471637738776292</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>109</v>
-      </c>
-      <c r="B17" t="s">
-        <v>110</v>
-      </c>
-    </row>
+    <row r="17" spans="1:29" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="18" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>104</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>136</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M19" t="s">
         <v>120</v>
       </c>
-      <c r="T18" t="s">
+      <c r="T19" t="s">
         <v>121</v>
       </c>
-      <c r="V18" t="s">
+      <c r="V19" t="s">
         <v>122</v>
       </c>
-      <c r="AC18" t="s">
+      <c r="AC19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>116</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>135</v>
       </c>
-      <c r="C19">
-        <f>SUM(C32:C37)</f>
+      <c r="C20">
+        <f>SUM(C33:C38)</f>
         <v>3542</v>
       </c>
-      <c r="D19">
-        <f t="shared" ref="D19:J19" si="7">SUM(D32:D37)</f>
+      <c r="D20">
+        <f t="shared" ref="D20:J20" si="7">SUM(D33:D38)</f>
         <v>7111</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <f t="shared" si="7"/>
         <v>10767</v>
       </c>
-      <c r="F19">
+      <c r="F20">
         <f t="shared" si="7"/>
         <v>7113</v>
       </c>
-      <c r="G19">
+      <c r="G20">
         <f t="shared" si="7"/>
         <v>7111</v>
       </c>
-      <c r="H19">
+      <c r="H20">
         <f t="shared" si="7"/>
         <v>20799</v>
       </c>
-      <c r="I19">
+      <c r="I20">
         <f t="shared" si="7"/>
         <v>20799</v>
       </c>
-      <c r="J19">
+      <c r="J20">
         <f t="shared" si="7"/>
         <v>10313</v>
       </c>
-      <c r="K19">
-        <f t="shared" ref="K19" si="8">SUM(K32:K37)</f>
+      <c r="K20">
+        <f t="shared" ref="K20" si="8">SUM(K33:K38)</f>
         <v>23265</v>
       </c>
-      <c r="M19" cm="1">
-        <f t="array" ref="M19:S25">TRANSPOSE(D19:J25)</f>
+      <c r="M20" cm="1">
+        <f t="array" ref="M20:S26">TRANSPOSE(D20:J26)</f>
         <v>7111</v>
       </c>
-      <c r="N19">
+      <c r="N20">
         <v>32838</v>
       </c>
-      <c r="O19">
+      <c r="O20">
         <v>66218</v>
       </c>
-      <c r="P19">
+      <c r="P20">
         <v>8076</v>
       </c>
-      <c r="Q19">
+      <c r="Q20">
         <v>8754</v>
       </c>
-      <c r="R19">
+      <c r="R20">
         <v>136</v>
       </c>
-      <c r="S19">
-        <v>1</v>
-      </c>
-      <c r="T19" cm="1">
-        <f t="array" ref="T19:T25">TRANSPOSE(D4:J4)</f>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20" cm="1">
+        <f t="array" ref="T20:T26">TRANSPOSE(D4:J4)</f>
         <v>180167</v>
       </c>
-      <c r="V19" cm="1">
-        <f t="array" ref="V19:AB25">MINVERSE(_xlfn.ANCHORARRAY(M19))</f>
+      <c r="V20" cm="1">
+        <f t="array" ref="V20:AB26">MINVERSE(_xlfn.ANCHORARRAY(M20))</f>
         <v>-3.635087081951479E-2</v>
       </c>
-      <c r="W19">
+      <c r="W20">
         <v>3.3922861115084674E-4</v>
       </c>
-      <c r="X19">
+      <c r="X20">
         <v>3.6263097317328408E-2</v>
       </c>
-      <c r="Y19">
+      <c r="Y20">
         <v>-8.537532976016373E-5</v>
       </c>
-      <c r="Z19">
+      <c r="Z20">
         <v>7.4902649042440746E-5</v>
       </c>
-      <c r="AA19">
+      <c r="AA20">
         <v>-5.4013706069903682E-5</v>
       </c>
-      <c r="AB19">
+      <c r="AB20">
         <v>-1.8696872217683933E-4</v>
       </c>
-      <c r="AC19" cm="1">
-        <f t="array" ref="AC19:AC25">MMULT(_xlfn.ANCHORARRAY(V19),_xlfn.ANCHORARRAY(T19))</f>
+      <c r="AC20" cm="1">
+        <f t="array" ref="AC20:AC26">MMULT(_xlfn.ANCHORARRAY(V20),_xlfn.ANCHORARRAY(T20))</f>
         <v>5.1005820389660883</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>56</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <f>SUM(C55,C46,C56)</f>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <f>SUM(C56,C47,C57)</f>
         <v>26340</v>
       </c>
-      <c r="D20">
-        <f t="shared" ref="D20:J20" si="9">SUM(D55,D46,D56)</f>
+      <c r="D21">
+        <f t="shared" ref="D21:J21" si="9">SUM(D56,D47,D57)</f>
         <v>32838</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <f t="shared" si="9"/>
         <v>36380</v>
       </c>
-      <c r="F20">
+      <c r="F21">
         <f t="shared" si="9"/>
         <v>32838</v>
       </c>
-      <c r="G20">
+      <c r="G21">
         <f t="shared" si="9"/>
         <v>70642</v>
       </c>
-      <c r="H20">
+      <c r="H21">
         <f t="shared" si="9"/>
         <v>114964</v>
       </c>
-      <c r="I20">
+      <c r="I21">
         <f t="shared" si="9"/>
         <v>73902</v>
       </c>
-      <c r="J20">
+      <c r="J21">
         <f t="shared" si="9"/>
         <v>43040</v>
       </c>
-      <c r="K20">
-        <f t="shared" ref="K20" si="10">SUM(K55,K46,K56)</f>
+      <c r="K21">
+        <f t="shared" ref="K21" si="10">SUM(K56,K47,K57)</f>
         <v>46955</v>
       </c>
-      <c r="M20">
+      <c r="M21">
         <v>10767</v>
       </c>
-      <c r="N20">
+      <c r="N21">
         <v>36380</v>
       </c>
-      <c r="O20">
+      <c r="O21">
         <v>76950</v>
       </c>
-      <c r="P20">
+      <c r="P21">
         <v>11732</v>
       </c>
-      <c r="Q20">
+      <c r="Q21">
         <v>8754</v>
       </c>
-      <c r="R20">
+      <c r="R21">
         <v>254</v>
       </c>
-      <c r="S20">
-        <v>1</v>
-      </c>
-      <c r="T20">
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
         <v>216495</v>
       </c>
-      <c r="V20">
+      <c r="V21">
         <v>3.9324532784843887E-2</v>
       </c>
-      <c r="W20">
+      <c r="W21">
         <v>-1.7838593987774123E-4</v>
       </c>
-      <c r="X20">
+      <c r="X21">
         <v>-3.933382198221004E-2</v>
       </c>
-      <c r="Y20">
+      <c r="Y21">
         <v>7.3872310242267076E-6</v>
       </c>
-      <c r="Z20">
+      <c r="Z21">
         <v>-2.2860238881440793E-5</v>
       </c>
-      <c r="AA20">
+      <c r="AA21">
         <v>3.750498086523561E-5</v>
       </c>
-      <c r="AB20">
+      <c r="AB21">
         <v>1.6564316423587071E-4</v>
       </c>
-      <c r="AC20">
+      <c r="AC21">
         <v>-0.11675093523181346</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>117</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>1.55</v>
       </c>
-      <c r="C21">
-        <f>SUM(C38:C42)</f>
+      <c r="C22">
+        <f>SUM(C39:C43)</f>
         <v>23130</v>
       </c>
-      <c r="D21">
-        <f t="shared" ref="D21:J21" si="11">SUM(D38:D42)</f>
+      <c r="D22">
+        <f t="shared" ref="D22:J22" si="11">SUM(D39:D43)</f>
         <v>66218</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <f t="shared" si="11"/>
         <v>76950</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <f t="shared" si="11"/>
         <v>66220</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <f t="shared" si="11"/>
         <v>136010</v>
       </c>
-      <c r="H21">
+      <c r="H22">
         <f t="shared" si="11"/>
         <v>165454</v>
       </c>
-      <c r="I21">
+      <c r="I22">
         <f t="shared" si="11"/>
         <v>148346</v>
       </c>
-      <c r="J21">
+      <c r="J22">
         <f t="shared" si="11"/>
         <v>70238</v>
       </c>
-      <c r="K21">
-        <f t="shared" ref="K21" si="12">SUM(K38:K42)</f>
+      <c r="K22">
+        <f t="shared" ref="K22" si="12">SUM(K39:K43)</f>
         <v>62288</v>
       </c>
-      <c r="M21">
+      <c r="M22">
         <v>7113</v>
       </c>
-      <c r="N21">
+      <c r="N22">
         <v>32838</v>
       </c>
-      <c r="O21">
+      <c r="O22">
         <v>66220</v>
       </c>
-      <c r="P21">
+      <c r="P22">
         <v>8076</v>
       </c>
-      <c r="Q21">
+      <c r="Q22">
         <v>8754</v>
       </c>
-      <c r="R21">
+      <c r="R22">
         <v>138</v>
       </c>
-      <c r="S21">
-        <v>1</v>
-      </c>
-      <c r="T21">
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22">
         <v>180181</v>
       </c>
-      <c r="V21">
+      <c r="V22">
         <v>-1.361724196571419E-2</v>
       </c>
-      <c r="W21">
+      <c r="W22">
         <v>3.26543015085874E-5</v>
       </c>
-      <c r="X21">
+      <c r="X22">
         <v>1.3624344241461816E-2</v>
       </c>
-      <c r="Y21">
+      <c r="Y22">
         <v>1.0534513201513464E-5</v>
       </c>
-      <c r="Z21">
+      <c r="Z22">
         <v>-1.0525039752714027E-6</v>
       </c>
-      <c r="AA21">
+      <c r="AA22">
         <v>2.4256926885382997E-6</v>
       </c>
-      <c r="AB21">
+      <c r="AB22">
         <v>-5.1664279170991959E-5</v>
       </c>
-      <c r="AC21">
+      <c r="AC22">
         <v>1.8749830109410635</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>118</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <v>1.55</v>
       </c>
-      <c r="C22">
-        <f>SUM(C43:C45)</f>
+      <c r="C23">
+        <f>SUM(C44:C46)</f>
         <v>4022</v>
       </c>
-      <c r="D22">
-        <f t="shared" ref="D22:J22" si="13">SUM(D43:D45)</f>
+      <c r="D23">
+        <f t="shared" ref="D23:J23" si="13">SUM(D44:D46)</f>
         <v>8076</v>
       </c>
-      <c r="E22">
+      <c r="E23">
         <f t="shared" si="13"/>
         <v>11732</v>
       </c>
-      <c r="F22">
+      <c r="F23">
         <f t="shared" si="13"/>
         <v>8076</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <f t="shared" si="13"/>
         <v>16800</v>
       </c>
-      <c r="H22">
+      <c r="H23">
         <f t="shared" si="13"/>
         <v>11498</v>
       </c>
-      <c r="I22">
+      <c r="I23">
         <f t="shared" si="13"/>
         <v>8078</v>
       </c>
-      <c r="J22">
+      <c r="J23">
         <f t="shared" si="13"/>
         <v>12096</v>
       </c>
-      <c r="K22">
-        <f t="shared" ref="K22" si="14">SUM(K43:K45)</f>
+      <c r="K23">
+        <f t="shared" ref="K23" si="14">SUM(K44:K46)</f>
         <v>7586</v>
       </c>
-      <c r="M22">
+      <c r="M23">
         <v>7111</v>
       </c>
-      <c r="N22">
+      <c r="N23">
         <v>70642</v>
       </c>
-      <c r="O22">
+      <c r="O23">
         <v>136010</v>
       </c>
-      <c r="P22">
+      <c r="P23">
         <v>16800</v>
       </c>
-      <c r="Q22">
+      <c r="Q23">
         <v>26202</v>
       </c>
-      <c r="R22">
+      <c r="R23">
         <v>136</v>
       </c>
-      <c r="S22">
-        <v>1</v>
-      </c>
-      <c r="T22">
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="T23">
         <v>357555</v>
       </c>
-      <c r="V22">
+      <c r="V23">
         <v>5.2476830432061736E-2</v>
       </c>
-      <c r="W22">
+      <c r="W23">
         <v>2.3265704754675745E-5</v>
       </c>
-      <c r="X22">
+      <c r="X23">
         <v>-5.2677032447099745E-2</v>
       </c>
-      <c r="Y22">
+      <c r="Y23">
         <v>4.4879382188945695E-5</v>
       </c>
-      <c r="Z22">
+      <c r="Z23">
         <v>-4.7282092177396974E-5</v>
       </c>
-      <c r="AA22">
+      <c r="AA23">
         <v>8.8926552665522262E-6</v>
       </c>
-      <c r="AB22">
+      <c r="AB23">
         <v>1.7044636500523016E-4</v>
       </c>
-      <c r="AC22">
+      <c r="AC23">
         <v>-0.55563378539225283</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>126</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <f>SUM(C51,C60,C61:C64,C52:C54,C57,C28)</f>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <f>SUM(C52,C61,C62:C65,C53:C55,C58,C29)</f>
         <v>14329</v>
       </c>
-      <c r="D23">
-        <f t="shared" ref="D23:J23" si="15">SUM(D51,D60,D61:D64,D52:D54,D57)</f>
+      <c r="D24">
+        <f t="shared" ref="D24:J24" si="15">SUM(D52,D61,D62:D65,D53:D55,D58)</f>
         <v>8754</v>
       </c>
-      <c r="E23">
+      <c r="E24">
         <f t="shared" si="15"/>
         <v>8754</v>
       </c>
-      <c r="F23">
+      <c r="F24">
         <f t="shared" si="15"/>
         <v>8754</v>
       </c>
-      <c r="G23">
+      <c r="G24">
         <f t="shared" si="15"/>
         <v>26202</v>
       </c>
-      <c r="H23">
+      <c r="H24">
         <f t="shared" si="15"/>
         <v>36130</v>
       </c>
-      <c r="I23">
+      <c r="I24">
         <f t="shared" si="15"/>
         <v>8754</v>
       </c>
-      <c r="J23">
+      <c r="J24">
         <f t="shared" si="15"/>
         <v>11754</v>
       </c>
-      <c r="K23">
-        <f t="shared" ref="K23" si="16">SUM(K51,K60,K61:K64,K52:K54,K57)</f>
+      <c r="K24">
+        <f t="shared" ref="K24" si="16">SUM(K52,K61,K62:K65,K53:K55,K58)</f>
         <v>49216</v>
       </c>
-      <c r="M23">
+      <c r="M24">
         <v>20799</v>
       </c>
-      <c r="N23">
+      <c r="N24">
         <v>114964</v>
       </c>
-      <c r="O23">
+      <c r="O24">
         <v>165454</v>
       </c>
-      <c r="P23">
+      <c r="P24">
         <v>11498</v>
       </c>
-      <c r="Q23">
+      <c r="Q24">
         <v>36130</v>
       </c>
-      <c r="R23">
+      <c r="R24">
         <v>136</v>
       </c>
-      <c r="S23">
-        <v>1</v>
-      </c>
-      <c r="T23">
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24">
         <v>512095</v>
       </c>
-      <c r="V23">
+      <c r="V24">
         <v>-5.7029914879437184E-2</v>
       </c>
-      <c r="W23">
+      <c r="W24">
         <v>2.4425281132341858E-4</v>
       </c>
-      <c r="X23">
+      <c r="X24">
         <v>5.7064420219157697E-2</v>
       </c>
-      <c r="Y23">
+      <c r="Y24">
         <v>-2.3270252018354897E-5</v>
       </c>
-      <c r="Z23">
+      <c r="Z24">
         <v>7.738157956623914E-5</v>
       </c>
-      <c r="AA23">
+      <c r="AA24">
         <v>-9.5409890262106474E-5</v>
       </c>
-      <c r="AB23">
+      <c r="AB24">
         <v>-2.3745958832970047E-4</v>
       </c>
-      <c r="AC23">
+      <c r="AC24">
         <v>3.197511875270358</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>124</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <f>SUM(C30:C31, C29,C65:C68,C58:C59)</f>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <f>SUM(C31:C32, C30,C66:C69,C59:C60)</f>
         <v>67</v>
       </c>
-      <c r="D24">
-        <f t="shared" ref="D24:J24" si="17">SUM(D30:D31, D29,D65:D68,D58:D59)</f>
+      <c r="D25">
+        <f t="shared" ref="D25:J25" si="17">SUM(D31:D32, D30,D66:D69,D59:D60)</f>
         <v>136</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <f t="shared" si="17"/>
         <v>254</v>
       </c>
-      <c r="F24">
+      <c r="F25">
         <f t="shared" si="17"/>
         <v>138</v>
       </c>
-      <c r="G24">
+      <c r="G25">
         <f t="shared" si="17"/>
         <v>136</v>
       </c>
-      <c r="H24">
+      <c r="H25">
         <f t="shared" si="17"/>
         <v>136</v>
       </c>
-      <c r="I24">
+      <c r="I25">
         <f t="shared" si="17"/>
         <v>136</v>
       </c>
-      <c r="J24">
+      <c r="J25">
         <f t="shared" si="17"/>
         <v>738</v>
       </c>
-      <c r="K24">
-        <f t="shared" ref="K24" si="18">SUM(K30:K31, K29,K65:K68,K58:K59)</f>
+      <c r="K25">
+        <f t="shared" ref="K25" si="18">SUM(K31:K32, K30,K66:K69,K59:K60)</f>
         <v>2716</v>
       </c>
-      <c r="M24">
+      <c r="M25">
         <v>20799</v>
       </c>
-      <c r="N24">
+      <c r="N25">
         <v>73902</v>
       </c>
-      <c r="O24">
+      <c r="O25">
         <v>148346</v>
       </c>
-      <c r="P24">
+      <c r="P25">
         <v>8078</v>
       </c>
-      <c r="Q24">
+      <c r="Q25">
         <v>8754</v>
       </c>
-      <c r="R24">
+      <c r="R25">
         <v>136</v>
       </c>
-      <c r="S24">
-        <v>1</v>
-      </c>
-      <c r="T24">
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="T25">
         <v>399177</v>
       </c>
-      <c r="V24">
+      <c r="V25">
         <v>-0.4500318872147781</v>
       </c>
-      <c r="W24">
+      <c r="W25">
         <v>-3.7188291265925137E-4</v>
       </c>
-      <c r="X24">
+      <c r="X25">
         <v>0.45011255844121684</v>
       </c>
-      <c r="Y24">
+      <c r="Y25">
         <v>7.484081655864177E-5</v>
       </c>
-      <c r="Z24">
+      <c r="Z25">
         <v>-7.3850145067154652E-5</v>
       </c>
-      <c r="AA24">
+      <c r="AA25">
         <v>5.1588013381318136E-5</v>
       </c>
-      <c r="AB24">
+      <c r="AB25">
         <v>2.3863300134775947E-4</v>
       </c>
-      <c r="AC24">
+      <c r="AC25">
         <v>2.4434950113864318E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>125</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>2863</v>
       </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="I25">
-        <v>1</v>
-      </c>
-      <c r="J25">
-        <v>1</v>
-      </c>
-      <c r="K25">
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
         <v>2</v>
       </c>
-      <c r="M25">
+      <c r="M26">
         <v>10313</v>
       </c>
-      <c r="N25">
+      <c r="N26">
         <v>43040</v>
       </c>
-      <c r="O25">
+      <c r="O26">
         <v>70238</v>
       </c>
-      <c r="P25">
+      <c r="P26">
         <v>12096</v>
       </c>
-      <c r="Q25">
+      <c r="Q26">
         <v>11754</v>
       </c>
-      <c r="R25">
+      <c r="R26">
         <v>738</v>
       </c>
-      <c r="S25">
-        <v>1</v>
-      </c>
-      <c r="T25">
+      <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26">
         <v>210219</v>
       </c>
-      <c r="V25">
+      <c r="V26">
         <v>6.4998922410006674</v>
       </c>
-      <c r="W25">
+      <c r="W26">
         <v>-0.99222656328635406</v>
       </c>
-      <c r="X25">
+      <c r="X26">
         <v>-3.7371942565618377</v>
       </c>
-      <c r="Y25">
+      <c r="Y26">
         <v>-0.50196877306807286</v>
       </c>
-      <c r="Z25">
+      <c r="Z26">
         <v>2.2419439134118537E-3</v>
       </c>
-      <c r="AA25">
+      <c r="AA26">
         <v>-0.2517364906372061</v>
       </c>
-      <c r="AB25">
+      <c r="AB26">
         <v>-1.9008101360608636E-2</v>
       </c>
-      <c r="AC25">
+      <c r="AC26">
         <v>65.95965508962945</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>96</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>97</v>
       </c>
-      <c r="M27" t="s">
+      <c r="M28" t="s">
         <v>128</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="Q28" t="s">
         <v>132</v>
       </c>
-      <c r="R27" t="s">
+      <c r="R28" t="s">
         <v>120</v>
       </c>
-      <c r="V27" t="s">
+      <c r="V28" t="s">
         <v>122</v>
       </c>
-      <c r="Z27" t="s">
+      <c r="Z28" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28">
-        <v>9967</v>
-      </c>
-      <c r="D28">
-        <v>4</v>
-      </c>
-      <c r="E28">
-        <v>4</v>
-      </c>
-      <c r="F28">
-        <v>4</v>
-      </c>
-      <c r="G28">
-        <v>4</v>
-      </c>
-      <c r="H28">
-        <v>4</v>
-      </c>
-      <c r="I28">
-        <v>4</v>
-      </c>
-      <c r="J28">
-        <v>204</v>
-      </c>
-      <c r="K28">
-        <v>4</v>
-      </c>
-      <c r="L28" t="s">
-        <v>129</v>
-      </c>
-      <c r="M28">
-        <f>D19</f>
-        <v>7111</v>
-      </c>
-      <c r="N28">
-        <f>E19</f>
-        <v>10767</v>
-      </c>
-      <c r="O28">
-        <f>G19</f>
-        <v>7111</v>
-      </c>
-      <c r="P28">
-        <f>J19</f>
-        <v>10313</v>
-      </c>
-      <c r="Q28">
-        <f>D4-D20-D23-D24</f>
-        <v>138439</v>
-      </c>
-      <c r="R28" cm="1">
-        <f t="array" ref="R28:U31">TRANSPOSE(M28:P31)</f>
-        <v>7111</v>
-      </c>
-      <c r="S28">
-        <v>66218</v>
-      </c>
-      <c r="T28">
-        <v>8076</v>
-      </c>
-      <c r="U28">
-        <v>1</v>
-      </c>
-      <c r="V28" cm="1">
-        <f t="array" ref="V28:Y31">MINVERSE(_xlfn.ANCHORARRAY(R28))</f>
-        <v>-1.459775187242437E-4</v>
-      </c>
-      <c r="W28">
-        <v>6.4553709512161193E-4</v>
-      </c>
-      <c r="X28">
-        <v>-7.4798920630780795E-5</v>
-      </c>
-      <c r="Y28">
-        <v>-4.247606557665874E-4</v>
-      </c>
-      <c r="Z28" cm="1">
-        <f t="array" ref="Z28:Z31">MMULT(_xlfn.ANCHORARRAY(V28),Q28:Q31)</f>
-        <v>5.0512537183762731</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>9967</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J29">
-        <v>1</v>
+        <v>204</v>
       </c>
       <c r="K29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M29">
-        <f>D21</f>
+        <f>D20</f>
+        <v>7111</v>
+      </c>
+      <c r="N29">
+        <f>E20</f>
+        <v>10767</v>
+      </c>
+      <c r="O29">
+        <f>G20</f>
+        <v>7111</v>
+      </c>
+      <c r="P29">
+        <f>J20</f>
+        <v>10313</v>
+      </c>
+      <c r="Q29">
+        <f>D4-D21-D24-D25</f>
+        <v>138439</v>
+      </c>
+      <c r="R29" cm="1">
+        <f t="array" ref="R29:U32">TRANSPOSE(M29:P32)</f>
+        <v>7111</v>
+      </c>
+      <c r="S29">
         <v>66218</v>
       </c>
-      <c r="N29">
-        <f>E21</f>
-        <v>76950</v>
-      </c>
-      <c r="O29">
-        <f>G21</f>
-        <v>136010</v>
-      </c>
-      <c r="P29">
-        <f>J21</f>
-        <v>70238</v>
-      </c>
-      <c r="Q29">
-        <f>E4-E20-E23-E24</f>
-        <v>171107</v>
-      </c>
-      <c r="R29">
-        <v>10767</v>
-      </c>
-      <c r="S29">
-        <v>76950</v>
-      </c>
       <c r="T29">
-        <v>11732</v>
+        <v>8076</v>
       </c>
       <c r="U29">
         <v>1</v>
       </c>
-      <c r="V29">
-        <v>2.550895020265855E-6</v>
+      <c r="V29" cm="1">
+        <f t="array" ref="V29:Y32">MINVERSE(_xlfn.ANCHORARRAY(R29))</f>
+        <v>-1.459775187242437E-4</v>
       </c>
       <c r="W29">
-        <v>7.3454505280007157E-5</v>
+        <v>6.4553709512161193E-4</v>
       </c>
       <c r="X29">
-        <v>7.8639536359250295E-6</v>
+        <v>-7.4798920630780795E-5</v>
       </c>
       <c r="Y29">
-        <v>-8.3869353936198078E-5</v>
-      </c>
-      <c r="Z29">
-        <v>1.9973743570092619</v>
+        <v>-4.247606557665874E-4</v>
+      </c>
+      <c r="Z29" cm="1">
+        <f t="array" ref="Z29:Z32">MMULT(_xlfn.ANCHORARRAY(V29),Q29:Q32)</f>
+        <v>5.0512537183762731</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>89</v>
       </c>
       <c r="C30">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>246</v>
+        <v>1</v>
       </c>
       <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30" t="s">
         <v>130</v>
-      </c>
-      <c r="G30">
-        <v>128</v>
-      </c>
-      <c r="H30">
-        <v>128</v>
-      </c>
-      <c r="I30">
-        <v>128</v>
-      </c>
-      <c r="J30">
-        <v>530</v>
-      </c>
-      <c r="K30">
-        <v>1418</v>
-      </c>
-      <c r="L30" t="s">
-        <v>131</v>
       </c>
       <c r="M30">
         <f>D22</f>
-        <v>8076</v>
+        <v>66218</v>
       </c>
       <c r="N30">
         <f>E22</f>
-        <v>11732</v>
+        <v>76950</v>
       </c>
       <c r="O30">
         <f>G22</f>
-        <v>16800</v>
+        <v>136010</v>
       </c>
       <c r="P30">
         <f>J22</f>
-        <v>12096</v>
+        <v>70238</v>
       </c>
       <c r="Q30">
-        <f>G4-G20-G23-G24</f>
-        <v>260575</v>
+        <f>E4-E21-E24-E25</f>
+        <v>171107</v>
       </c>
       <c r="R30">
-        <v>7111</v>
+        <v>10767</v>
       </c>
       <c r="S30">
-        <v>136010</v>
+        <v>76950</v>
       </c>
       <c r="T30">
-        <v>16800</v>
+        <v>11732</v>
       </c>
       <c r="U30">
         <v>1</v>
       </c>
       <c r="V30">
-        <v>-1.3503347836478616E-4</v>
+        <v>2.550895020265855E-6</v>
       </c>
       <c r="W30">
-        <v>-5.8763604224005726E-4</v>
+        <v>7.3454505280007157E-5</v>
       </c>
       <c r="X30">
-        <v>5.1714689115259085E-5</v>
+        <v>7.8639536359250295E-6</v>
       </c>
       <c r="Y30">
-        <v>6.7095483148958452E-4</v>
+        <v>-8.3869353936198078E-5</v>
       </c>
       <c r="Z30">
-        <v>-1.9789948560741237</v>
+        <v>1.9973743570092619</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="D31">
-        <v>6</v>
+        <v>128</v>
       </c>
       <c r="E31">
-        <v>6</v>
+        <v>246</v>
       </c>
       <c r="F31">
-        <v>6</v>
+        <v>130</v>
       </c>
       <c r="G31">
-        <v>6</v>
+        <v>128</v>
       </c>
       <c r="H31">
-        <v>6</v>
+        <v>128</v>
       </c>
       <c r="I31">
-        <v>6</v>
+        <v>128</v>
       </c>
       <c r="J31">
-        <v>206</v>
+        <v>530</v>
       </c>
       <c r="K31">
-        <v>1296</v>
+        <v>1418</v>
       </c>
       <c r="L31" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="M31">
-        <v>1</v>
+        <f>D23</f>
+        <v>8076</v>
       </c>
       <c r="N31">
-        <v>1</v>
+        <f>E23</f>
+        <v>11732</v>
       </c>
       <c r="O31">
-        <v>1</v>
+        <f>G23</f>
+        <v>16800</v>
       </c>
       <c r="P31">
-        <v>1</v>
+        <f>J23</f>
+        <v>12096</v>
       </c>
       <c r="Q31">
-        <f>J4-J20-J23-J24</f>
-        <v>154687</v>
+        <f>G4-G21-G24-G25</f>
+        <v>260575</v>
       </c>
       <c r="R31">
-        <v>10313</v>
+        <v>7111</v>
       </c>
       <c r="S31">
-        <v>70238</v>
+        <v>136010</v>
       </c>
       <c r="T31">
-        <v>12096</v>
+        <v>16800</v>
       </c>
       <c r="U31">
         <v>1</v>
       </c>
       <c r="V31">
-        <v>2.9596613404701455</v>
+        <v>-1.3503347836478616E-4</v>
       </c>
       <c r="W31">
-        <v>-4.7086760369105942</v>
+        <v>-5.8763604224005726E-4</v>
       </c>
       <c r="X31">
-        <v>-0.4064879865530337</v>
+        <v>5.1714689115259085E-5</v>
       </c>
       <c r="Y31">
-        <v>3.1555026829934829</v>
+        <v>6.7095483148958452E-4</v>
       </c>
       <c r="Z31">
-        <v>-13760.237906158436</v>
+        <v>-1.9789948560741237</v>
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E32">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F32">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G32">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H32">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I32">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J32">
-        <v>2</v>
+        <v>206</v>
       </c>
       <c r="K32">
-        <v>7650</v>
+        <v>1296</v>
+      </c>
+      <c r="L32" t="s">
+        <v>125</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32">
+        <v>1</v>
+      </c>
+      <c r="Q32">
+        <f>J4-J21-J24-J25</f>
+        <v>154687</v>
+      </c>
+      <c r="R32">
+        <v>10313</v>
+      </c>
+      <c r="S32">
+        <v>70238</v>
+      </c>
+      <c r="T32">
+        <v>12096</v>
+      </c>
+      <c r="U32">
+        <v>1</v>
+      </c>
+      <c r="V32">
+        <v>2.9596613404701455</v>
+      </c>
+      <c r="W32">
+        <v>-4.7086760369105942</v>
+      </c>
+      <c r="X32">
+        <v>-0.4064879865530337</v>
+      </c>
+      <c r="Y32">
+        <v>3.1555026829934829</v>
+      </c>
+      <c r="Z32">
+        <v>-13760.237906158436</v>
       </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J33">
-        <v>404</v>
+        <v>2</v>
       </c>
       <c r="K33">
-        <v>7332</v>
-      </c>
-      <c r="M33" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>132</v>
-      </c>
-      <c r="S33" t="s">
-        <v>120</v>
-      </c>
-      <c r="V33" t="s">
-        <v>122</v>
-      </c>
-      <c r="Z33" t="s">
-        <v>123</v>
+        <v>7650</v>
       </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C34">
-        <v>1829</v>
+        <v>0</v>
       </c>
       <c r="D34">
-        <v>3657</v>
+        <v>4</v>
       </c>
       <c r="E34">
-        <v>7313</v>
+        <v>4</v>
       </c>
       <c r="F34">
-        <v>3659</v>
+        <v>4</v>
       </c>
       <c r="G34">
-        <v>3657</v>
+        <v>4</v>
       </c>
       <c r="H34">
-        <v>3657</v>
+        <v>4</v>
       </c>
       <c r="I34">
-        <v>3657</v>
+        <v>4</v>
       </c>
       <c r="J34">
-        <v>3657</v>
+        <v>404</v>
       </c>
       <c r="K34">
-        <v>3657</v>
-      </c>
-      <c r="L34" t="s">
-        <v>129</v>
-      </c>
-      <c r="M34">
-        <f>D19</f>
-        <v>7111</v>
-      </c>
-      <c r="N34">
-        <f>E19</f>
-        <v>10767</v>
-      </c>
-      <c r="O34">
-        <f>G19</f>
-        <v>7111</v>
-      </c>
-      <c r="Q34">
-        <f>D4-D20-D23-D24</f>
-        <v>138439</v>
-      </c>
-      <c r="S34" cm="1">
-        <f t="array" ref="S34:U36">TRANSPOSE(M34:O36)</f>
-        <v>7111</v>
-      </c>
-      <c r="T34">
-        <v>74294</v>
-      </c>
-      <c r="U34">
-        <v>1</v>
-      </c>
-      <c r="V34" cm="1">
-        <f t="array" ref="V34:X36">MINVERSE(_xlfn.ANCHORARRAY(S34))</f>
-        <v>-2.2340008915937691E-4</v>
-      </c>
-      <c r="W34">
-        <v>2.7352297592997811E-4</v>
-      </c>
-      <c r="X34">
-        <v>-5.0122886770601223E-5</v>
-      </c>
-      <c r="Z34" cm="1">
-        <f t="array" ref="Z34:Z36">MMULT(_xlfn.ANCHORARRAY(V34),Q34:Q36)</f>
-        <v>2.813639679066366</v>
+        <v>7332</v>
+      </c>
+      <c r="M34" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>132</v>
+      </c>
+      <c r="S34" t="s">
+        <v>120</v>
+      </c>
+      <c r="V34" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35">
+        <v>1829</v>
+      </c>
+      <c r="D35">
+        <v>3657</v>
+      </c>
+      <c r="E35">
+        <v>7313</v>
+      </c>
+      <c r="F35">
+        <v>3659</v>
+      </c>
+      <c r="G35">
+        <v>3657</v>
+      </c>
+      <c r="H35">
+        <v>3657</v>
+      </c>
+      <c r="I35">
+        <v>3657</v>
+      </c>
+      <c r="J35">
+        <v>3657</v>
+      </c>
+      <c r="K35">
+        <v>3657</v>
+      </c>
+      <c r="L35" t="s">
+        <v>129</v>
+      </c>
+      <c r="M35">
+        <f>D20</f>
+        <v>7111</v>
+      </c>
+      <c r="N35">
+        <f>E20</f>
+        <v>10767</v>
+      </c>
+      <c r="O35">
+        <f>G20</f>
+        <v>7111</v>
+      </c>
+      <c r="Q35">
+        <f>D4-D21-D24-D25</f>
+        <v>138439</v>
+      </c>
+      <c r="S35" cm="1">
+        <f t="array" ref="S35:U37">TRANSPOSE(M35:O37)</f>
+        <v>7111</v>
+      </c>
+      <c r="T35">
+        <v>74294</v>
+      </c>
+      <c r="U35">
+        <v>1</v>
+      </c>
+      <c r="V35" cm="1">
+        <f t="array" ref="V35:X37">MINVERSE(_xlfn.ANCHORARRAY(S35))</f>
+        <v>-2.2340008915937691E-4</v>
+      </c>
+      <c r="W35">
+        <v>2.7352297592997811E-4</v>
+      </c>
+      <c r="X35">
+        <v>-5.0122886770601223E-5</v>
+      </c>
+      <c r="Z35" cm="1">
+        <f t="array" ref="Z35:Z37">MMULT(_xlfn.ANCHORARRAY(V35),Q35:Q37)</f>
+        <v>2.813639679066366</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>71</v>
       </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="J35">
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
         <v>202</v>
       </c>
-      <c r="K35">
+      <c r="K36">
         <v>102</v>
       </c>
-      <c r="L35" t="s">
+      <c r="L36" t="s">
         <v>134</v>
       </c>
-      <c r="M35">
-        <f>M29+M30</f>
+      <c r="M36">
+        <f>M30+M31</f>
         <v>74294</v>
       </c>
-      <c r="N35">
-        <f t="shared" ref="N35:O35" si="19">N29+N30</f>
+      <c r="N36">
+        <f t="shared" ref="N36:O36" si="19">N30+N31</f>
         <v>88682</v>
       </c>
-      <c r="O35">
+      <c r="O36">
         <f t="shared" si="19"/>
         <v>152810</v>
       </c>
-      <c r="Q35">
-        <f>E4-E20-E23-E24</f>
+      <c r="Q36">
+        <f>E4-E21-E24-E25</f>
         <v>171107</v>
       </c>
-      <c r="S35">
+      <c r="S36">
         <v>10767</v>
       </c>
-      <c r="T35">
+      <c r="T36">
         <v>88682</v>
       </c>
-      <c r="U35">
-        <v>1</v>
-      </c>
-      <c r="V35">
+      <c r="U36">
+        <v>1</v>
+      </c>
+      <c r="V36">
         <v>-1.2736257578073259E-5</v>
       </c>
-      <c r="W35">
-        <v>0</v>
-      </c>
-      <c r="X35">
+      <c r="W36">
+        <v>0</v>
+      </c>
+      <c r="X36">
         <v>1.2736257578073259E-5</v>
       </c>
-      <c r="Z35">
+      <c r="Z36">
         <v>1.5555555555555556</v>
-      </c>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <v>22</v>
-      </c>
-      <c r="E36">
-        <v>22</v>
-      </c>
-      <c r="F36">
-        <v>22</v>
-      </c>
-      <c r="G36">
-        <v>22</v>
-      </c>
-      <c r="H36">
-        <v>22</v>
-      </c>
-      <c r="I36">
-        <v>22</v>
-      </c>
-      <c r="J36">
-        <v>2222</v>
-      </c>
-      <c r="K36">
-        <v>662</v>
-      </c>
-      <c r="L36" t="s">
-        <v>125</v>
-      </c>
-      <c r="M36">
-        <v>1</v>
-      </c>
-      <c r="N36">
-        <v>1</v>
-      </c>
-      <c r="O36">
-        <v>1</v>
-      </c>
-      <c r="Q36">
-        <f>G4-G20-G23-G24</f>
-        <v>260575</v>
-      </c>
-      <c r="S36">
-        <v>7111</v>
-      </c>
-      <c r="T36">
-        <v>152810</v>
-      </c>
-      <c r="U36">
-        <v>1</v>
-      </c>
-      <c r="V36">
-        <v>3.5348255545177039</v>
-      </c>
-      <c r="W36">
-        <v>-1.9450218818380745</v>
-      </c>
-      <c r="X36">
-        <v>-0.58980367267962941</v>
-      </c>
-      <c r="Z36">
-        <v>2862.7637977146078</v>
       </c>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C37">
-        <v>1711</v>
+        <v>0</v>
       </c>
       <c r="D37">
-        <v>3426</v>
+        <v>22</v>
       </c>
       <c r="E37">
-        <v>3426</v>
+        <v>22</v>
       </c>
       <c r="F37">
-        <v>3426</v>
+        <v>22</v>
       </c>
       <c r="G37">
-        <v>3426</v>
+        <v>22</v>
       </c>
       <c r="H37">
-        <v>17114</v>
+        <v>22</v>
       </c>
       <c r="I37">
-        <v>17114</v>
+        <v>22</v>
       </c>
       <c r="J37">
-        <v>3826</v>
+        <v>2222</v>
       </c>
       <c r="K37">
-        <v>3862</v>
+        <v>662</v>
+      </c>
+      <c r="L37" t="s">
+        <v>125</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="O37">
+        <v>1</v>
+      </c>
+      <c r="Q37">
+        <f>G4-G21-G24-G25</f>
+        <v>260575</v>
+      </c>
+      <c r="S37">
+        <v>7111</v>
+      </c>
+      <c r="T37">
+        <v>152810</v>
+      </c>
+      <c r="U37">
+        <v>1</v>
+      </c>
+      <c r="V37">
+        <v>3.5348255545177039</v>
+      </c>
+      <c r="W37">
+        <v>-1.9450218818380745</v>
+      </c>
+      <c r="X37">
+        <v>-0.58980367267962941</v>
+      </c>
+      <c r="Z37">
+        <v>2862.7637977146078</v>
       </c>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>1711</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>3426</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>3426</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>3426</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>3426</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>17114</v>
       </c>
       <c r="I38">
-        <v>0</v>
+        <v>17114</v>
       </c>
       <c r="J38">
-        <v>0</v>
+        <v>3826</v>
       </c>
       <c r="K38">
-        <v>0</v>
+        <v>3862</v>
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -3225,284 +3198,287 @@
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C40">
-        <v>15346</v>
+        <v>0</v>
       </c>
       <c r="D40">
-        <v>50644</v>
+        <v>0</v>
       </c>
       <c r="E40">
-        <v>61376</v>
+        <v>0</v>
       </c>
       <c r="F40">
-        <v>50646</v>
+        <v>0</v>
       </c>
       <c r="G40">
-        <v>102988</v>
+        <v>0</v>
       </c>
       <c r="H40">
-        <v>122504</v>
+        <v>0</v>
       </c>
       <c r="I40">
-        <v>105396</v>
+        <v>0</v>
       </c>
       <c r="J40">
-        <v>54064</v>
+        <v>0</v>
       </c>
       <c r="K40">
-        <v>47696</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C41">
-        <v>7784</v>
+        <v>15346</v>
       </c>
       <c r="D41">
-        <v>15574</v>
+        <v>50644</v>
       </c>
       <c r="E41">
-        <v>15574</v>
+        <v>61376</v>
       </c>
       <c r="F41">
-        <v>15574</v>
+        <v>50646</v>
       </c>
       <c r="G41">
-        <v>33022</v>
+        <v>102988</v>
       </c>
       <c r="H41">
-        <v>42950</v>
+        <v>122504</v>
       </c>
       <c r="I41">
-        <v>42950</v>
+        <v>105396</v>
       </c>
       <c r="J41">
-        <v>16174</v>
+        <v>54064</v>
       </c>
       <c r="K41">
-        <v>6</v>
+        <v>47696</v>
       </c>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>7784</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>15574</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>15574</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>15574</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>33022</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>42950</v>
       </c>
       <c r="I42">
-        <v>0</v>
+        <v>42950</v>
       </c>
       <c r="J42">
-        <v>0</v>
+        <v>16174</v>
       </c>
       <c r="K42">
-        <v>14586</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C43">
-        <v>2181</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>4368</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>4368</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>4368</v>
+        <v>0</v>
       </c>
       <c r="G43">
-        <v>13092</v>
+        <v>0</v>
       </c>
       <c r="H43">
-        <v>4368</v>
+        <v>0</v>
       </c>
       <c r="I43">
-        <v>4368</v>
+        <v>0</v>
       </c>
       <c r="J43">
-        <v>4968</v>
+        <v>0</v>
       </c>
       <c r="K43">
-        <v>6</v>
+        <v>14586</v>
       </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>2181</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>4368</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>4368</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>4368</v>
       </c>
       <c r="G44">
-        <v>0</v>
+        <v>13092</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>4368</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>4368</v>
       </c>
       <c r="J44">
-        <v>0</v>
+        <v>4968</v>
       </c>
       <c r="K44">
-        <v>3870</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C45">
-        <v>1841</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>3708</v>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>7364</v>
+        <v>0</v>
       </c>
       <c r="F45">
-        <v>3708</v>
+        <v>0</v>
       </c>
       <c r="G45">
-        <v>3708</v>
+        <v>0</v>
       </c>
       <c r="H45">
-        <v>7130</v>
+        <v>0</v>
       </c>
       <c r="I45">
-        <v>3710</v>
+        <v>0</v>
       </c>
       <c r="J45">
-        <v>7128</v>
+        <v>0</v>
       </c>
       <c r="K45">
-        <v>3710</v>
+        <v>3870</v>
       </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46">
+        <v>1841</v>
+      </c>
+      <c r="D46">
+        <v>3708</v>
+      </c>
+      <c r="E46">
+        <v>7364</v>
+      </c>
+      <c r="F46">
+        <v>3708</v>
+      </c>
+      <c r="G46">
+        <v>3708</v>
+      </c>
+      <c r="H46">
+        <v>7130</v>
+      </c>
+      <c r="I46">
+        <v>3710</v>
+      </c>
+      <c r="J46">
+        <v>7128</v>
+      </c>
+      <c r="K46">
+        <v>3710</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>78</v>
       </c>
-      <c r="C46">
+      <c r="C47">
         <v>16375</v>
       </c>
-      <c r="D46">
+      <c r="D47">
         <v>12898</v>
       </c>
-      <c r="E46">
+      <c r="E47">
         <v>16440</v>
       </c>
-      <c r="F46">
+      <c r="F47">
         <v>12898</v>
       </c>
-      <c r="G46">
+      <c r="G47">
         <v>24530</v>
       </c>
-      <c r="H46">
+      <c r="H47">
         <v>36850</v>
       </c>
-      <c r="I46">
+      <c r="I47">
         <v>26586</v>
       </c>
-      <c r="J46">
+      <c r="J47">
         <v>22100</v>
       </c>
-      <c r="K46">
+      <c r="K47">
         <v>20425</v>
-      </c>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>19</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="D47">
-        <v>0</v>
-      </c>
-      <c r="E47">
-        <v>0</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
-      <c r="I47">
-        <v>0</v>
-      </c>
-      <c r="J47">
-        <v>0</v>
-      </c>
-      <c r="K47">
-        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -3534,7 +3510,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -3566,109 +3542,106 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>22</v>
       </c>
-      <c r="C50">
-        <v>0</v>
-      </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="F50">
-        <v>0</v>
-      </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-      <c r="H50">
-        <v>0</v>
-      </c>
-      <c r="I50">
-        <v>0</v>
-      </c>
-      <c r="J50">
-        <v>0</v>
-      </c>
-      <c r="K50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B51" t="s">
-        <v>79</v>
-      </c>
       <c r="C51">
-        <v>2181</v>
+        <v>0</v>
       </c>
       <c r="D51">
-        <v>4370</v>
+        <v>0</v>
       </c>
       <c r="E51">
-        <v>4370</v>
+        <v>0</v>
       </c>
       <c r="F51">
-        <v>4370</v>
+        <v>0</v>
       </c>
       <c r="G51">
-        <v>13094</v>
+        <v>0</v>
       </c>
       <c r="H51">
-        <v>4370</v>
+        <v>0</v>
       </c>
       <c r="I51">
-        <v>4370</v>
+        <v>0</v>
       </c>
       <c r="J51">
-        <v>5170</v>
+        <v>0</v>
       </c>
       <c r="K51">
-        <v>6796</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B52" t="s">
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>2181</v>
       </c>
       <c r="D52">
-        <v>10</v>
+        <v>4370</v>
       </c>
       <c r="E52">
-        <v>10</v>
+        <v>4370</v>
       </c>
       <c r="F52">
-        <v>10</v>
+        <v>4370</v>
       </c>
       <c r="G52">
-        <v>10</v>
+        <v>13094</v>
       </c>
       <c r="H52">
-        <v>10</v>
+        <v>4370</v>
       </c>
       <c r="I52">
-        <v>10</v>
+        <v>4370</v>
       </c>
       <c r="J52">
-        <v>1010</v>
+        <v>5170</v>
       </c>
       <c r="K52">
-        <v>29330</v>
+        <v>6796</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B53" t="s">
         <v>119</v>
@@ -3677,33 +3650,33 @@
         <v>0</v>
       </c>
       <c r="D53">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E53">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F53">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G53">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H53">
-        <v>13694</v>
+        <v>10</v>
       </c>
       <c r="I53">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J53">
-        <v>606</v>
+        <v>1010</v>
       </c>
       <c r="K53">
-        <v>11742</v>
+        <v>29330</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B54" t="s">
         <v>119</v>
@@ -3712,141 +3685,141 @@
         <v>0</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G54">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H54">
-        <v>13688</v>
+        <v>13694</v>
       </c>
       <c r="I54">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J54">
-        <v>0</v>
+        <v>606</v>
       </c>
       <c r="K54">
-        <v>0</v>
+        <v>11742</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B55" t="s">
-        <v>56</v>
+        <v>119</v>
       </c>
       <c r="C55">
-        <v>9965</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>19936</v>
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>19936</v>
+        <v>0</v>
       </c>
       <c r="F55">
-        <v>19936</v>
+        <v>0</v>
       </c>
       <c r="G55">
-        <v>46108</v>
+        <v>0</v>
       </c>
       <c r="H55">
-        <v>64422</v>
+        <v>13688</v>
       </c>
       <c r="I55">
-        <v>47312</v>
+        <v>0</v>
       </c>
       <c r="J55">
-        <v>20536</v>
+        <v>0</v>
       </c>
       <c r="K55">
-        <v>25614</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>9965</v>
       </c>
       <c r="D56">
-        <v>4</v>
+        <v>19936</v>
       </c>
       <c r="E56">
-        <v>4</v>
+        <v>19936</v>
       </c>
       <c r="F56">
-        <v>4</v>
+        <v>19936</v>
       </c>
       <c r="G56">
-        <v>4</v>
+        <v>46108</v>
       </c>
       <c r="H56">
-        <v>13692</v>
+        <v>64422</v>
       </c>
       <c r="I56">
-        <v>4</v>
+        <v>47312</v>
       </c>
       <c r="J56">
-        <v>404</v>
+        <v>20536</v>
       </c>
       <c r="K56">
-        <v>916</v>
+        <v>25614</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B57" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>13692</v>
       </c>
       <c r="I57">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J57">
-        <v>0</v>
+        <v>404</v>
       </c>
       <c r="K57">
-        <v>0</v>
+        <v>916</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B58" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -3878,10 +3851,10 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -3913,80 +3886,80 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C60">
-        <v>2181</v>
+        <v>0</v>
       </c>
       <c r="D60">
-        <v>4364</v>
+        <v>0</v>
       </c>
       <c r="E60">
-        <v>4364</v>
+        <v>0</v>
       </c>
       <c r="F60">
-        <v>4364</v>
+        <v>0</v>
       </c>
       <c r="G60">
-        <v>13088</v>
+        <v>0</v>
       </c>
       <c r="H60">
-        <v>4364</v>
+        <v>0</v>
       </c>
       <c r="I60">
-        <v>4364</v>
+        <v>0</v>
       </c>
       <c r="J60">
-        <v>4564</v>
+        <v>0</v>
       </c>
       <c r="K60">
-        <v>1292</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>2181</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>4364</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>4364</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>4364</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>13088</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>4364</v>
       </c>
       <c r="I61">
-        <v>0</v>
+        <v>4364</v>
       </c>
       <c r="J61">
-        <v>0</v>
+        <v>4564</v>
       </c>
       <c r="K61">
-        <v>0</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -4018,80 +3991,80 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B63" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E63">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F63">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G63">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H63">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I63">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J63">
-        <v>404</v>
+        <v>0</v>
       </c>
       <c r="K63">
-        <v>56</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G64">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H64">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I64">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J64">
-        <v>0</v>
+        <v>404</v>
       </c>
       <c r="K64">
-        <v>0</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B65" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -4123,10 +4096,10 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B66" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -4158,77 +4131,80 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B67" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K67">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B68" t="s">
+        <v>76</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>1</v>
+      </c>
+      <c r="J68">
+        <v>1</v>
+      </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>77</v>
-      </c>
-      <c r="C68">
-        <v>0</v>
-      </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-      <c r="F68">
-        <v>0</v>
-      </c>
-      <c r="G68">
-        <v>0</v>
-      </c>
-      <c r="H68">
-        <v>0</v>
-      </c>
-      <c r="I68">
-        <v>0</v>
-      </c>
-      <c r="J68">
-        <v>0</v>
-      </c>
-      <c r="K68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>41</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -4260,7 +4236,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -4292,7 +4268,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -4324,7 +4300,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -4356,7 +4332,7 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -4388,7 +4364,7 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -4420,7 +4396,7 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -4452,7 +4428,7 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -4484,7 +4460,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -4516,7 +4492,7 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -4548,7 +4524,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -4580,7 +4556,7 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -4612,7 +4588,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -4644,33 +4620,65 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>53</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>54</v>
       </c>
-      <c r="C82">
-        <v>0</v>
-      </c>
-      <c r="D82">
-        <v>0</v>
-      </c>
-      <c r="E82">
-        <v>0</v>
-      </c>
-      <c r="F82">
-        <v>0</v>
-      </c>
-      <c r="G82">
-        <v>0</v>
-      </c>
-      <c r="H82">
-        <v>0</v>
-      </c>
-      <c r="I82">
-        <v>0</v>
-      </c>
-      <c r="J82">
-        <v>0</v>
-      </c>
-      <c r="K82">
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+      <c r="K83">
         <v>0</v>
       </c>
     </row>

</xml_diff>